<commit_message>
updated PV and electricity prices to latest data for 2019
</commit_message>
<xml_diff>
--- a/code/COSA_Data/historical_data.xlsx
+++ b/code/COSA_Data/historical_data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12160" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12163"/>
   </bookViews>
   <sheets>
     <sheet name="annual_data" sheetId="1" r:id="rId1"/>
@@ -25,8 +25,42 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Nunez-Jimenez  Alejandro</author>
+  </authors>
+  <commentList>
+    <comment ref="C33" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Nunez-Jimenez  Alejandro:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+NSR 2019, Average cost 10-30 kWp</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="124">
   <si>
     <t>source</t>
   </si>
@@ -390,6 +424,27 @@
   <si>
     <t>system_price_projection</t>
   </si>
+  <si>
+    <t>Av change last 5-years</t>
+  </si>
+  <si>
+    <t>Av 2015-2019</t>
+  </si>
+  <si>
+    <t>Av 2017-2019</t>
+  </si>
+  <si>
+    <t>Av 2016-2020</t>
+  </si>
+  <si>
+    <t>Av 2018-2020</t>
+  </si>
+  <si>
+    <t>Av all</t>
+  </si>
+  <si>
+    <t>Av bold</t>
+  </si>
 </sst>
 </file>
 
@@ -399,7 +454,7 @@
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -469,6 +524,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -484,12 +560,51 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -500,7 +615,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -564,6 +679,24 @@
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="10" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="13" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -830,7 +963,7 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>Projection (-5.1% p.a.)</c:v>
+            <c:v>Projection (-6.1% p.a.)</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
@@ -1007,55 +1140,55 @@
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="45"/>
                 <c:pt idx="28" formatCode="0.0000">
-                  <c:v>2.3725000000000001</c:v>
+                  <c:v>2.1840000000000002</c:v>
                 </c:pt>
                 <c:pt idx="29" formatCode="0.0000">
-                  <c:v>2.2515025</c:v>
+                  <c:v>2.0516034507602341</c:v>
                 </c:pt>
                 <c:pt idx="30" formatCode="0.0000">
-                  <c:v>2.1366758724999997</c:v>
+                  <c:v>1.9272329300234889</c:v>
                 </c:pt>
                 <c:pt idx="31" formatCode="0.0000">
-                  <c:v>2.0277054030024995</c:v>
+                  <c:v>1.8104018908676494</c:v>
                 </c:pt>
                 <c:pt idx="32" formatCode="0.0000">
-                  <c:v>1.9242924274493718</c:v>
+                  <c:v>1.7006532813951107</c:v>
                 </c:pt>
                 <c:pt idx="33" formatCode="0.0000">
-                  <c:v>1.8261535136494538</c:v>
+                  <c:v>1.5975577567110459</c:v>
                 </c:pt>
                 <c:pt idx="34" formatCode="0.0000">
-                  <c:v>1.7330196844533317</c:v>
+                  <c:v>1.5007119992935714</c:v>
                 </c:pt>
                 <c:pt idx="35" formatCode="0.0000">
-                  <c:v>1.6446356805462117</c:v>
+                  <c:v>1.4097371411849728</c:v>
                 </c:pt>
                 <c:pt idx="36" formatCode="0.0000">
-                  <c:v>1.5607592608383547</c:v>
+                  <c:v>1.3242772818314823</c:v>
                 </c:pt>
                 <c:pt idx="37" formatCode="0.0000">
-                  <c:v>1.4811605385355986</c:v>
+                  <c:v>1.2439980957732839</c:v>
                 </c:pt>
                 <c:pt idx="38" formatCode="0.0000">
-                  <c:v>1.4056213510702831</c:v>
+                  <c:v>1.1685855247379255</c:v>
                 </c:pt>
                 <c:pt idx="39" formatCode="0.0000">
-                  <c:v>1.3339346621656987</c:v>
+                  <c:v>1.0977445490205067</c:v>
                 </c:pt>
                 <c:pt idx="40" formatCode="0.0000">
-                  <c:v>1.2659039943952479</c:v>
+                  <c:v>1.0311980333441888</c:v>
                 </c:pt>
                 <c:pt idx="41" formatCode="0.0000">
-                  <c:v>1.2013428906810901</c:v>
+                  <c:v>0.96868564268594526</c:v>
                 </c:pt>
                 <c:pt idx="42" formatCode="0.0000">
-                  <c:v>1.1400744032563546</c:v>
+                  <c:v>0.90996282382618143</c:v>
                 </c:pt>
                 <c:pt idx="43" formatCode="0.0000">
-                  <c:v>1.0819306086902805</c:v>
+                  <c:v>0.85479984863796732</c:v>
                 </c:pt>
                 <c:pt idx="44" formatCode="0.0000">
-                  <c:v>1.026752147647076</c:v>
+                  <c:v>0.80298091537315908</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1115,7 +1248,7 @@
                 <a:cs typeface="DejaVu Sans" panose="020B0603030804020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="564089407"/>
@@ -1175,7 +1308,7 @@
                   <a:cs typeface="DejaVu Sans" panose="020B0603030804020204" pitchFamily="34" charset="0"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1207,7 +1340,7 @@
                 <a:cs typeface="DejaVu Sans" panose="020B0603030804020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="564079007"/>
@@ -1258,7 +1391,7 @@
               <a:cs typeface="DejaVu Sans" panose="020B0603030804020204" pitchFamily="34" charset="0"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1290,7 +1423,7 @@
           <a:cs typeface="DejaVu Sans" panose="020B0603030804020204" pitchFamily="34" charset="0"/>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1569,7 +1702,7 @@
                   <a:cs typeface="DejaVu Sans" panose="020B0603030804020204" pitchFamily="34" charset="0"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1601,7 +1734,7 @@
                 <a:cs typeface="DejaVu Sans" panose="020B0603030804020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="673718463"/>
@@ -1675,7 +1808,7 @@
                   <a:cs typeface="DejaVu Sans" panose="020B0603030804020204" pitchFamily="34" charset="0"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1707,7 +1840,7 @@
                 <a:cs typeface="DejaVu Sans" panose="020B0603030804020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="673724703"/>
@@ -1752,7 +1885,7 @@
           <a:cs typeface="DejaVu Sans" panose="020B0603030804020204" pitchFamily="34" charset="0"/>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2879,16 +3012,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>53</xdr:col>
-      <xdr:colOff>171450</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>51</xdr:col>
+      <xdr:colOff>1213368</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>177282</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>57</xdr:col>
-      <xdr:colOff>260350</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
+      <xdr:col>55</xdr:col>
+      <xdr:colOff>135942</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>85531</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2897,8 +3030,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="45935900" y="76200"/>
-          <a:ext cx="2527300" cy="825500"/>
+          <a:off x="63837327" y="7859486"/>
+          <a:ext cx="2701472" cy="1027922"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2940,13 +3073,16 @@
         <a:p>
           <a:r>
             <a:rPr lang="de-CH" sz="1400" b="0" i="0"/>
-            <a:t>Average 2014-2018 = +6.6%</a:t>
+            <a:t>Average 2017-2019 = +0.31%</a:t>
           </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="de-CH" sz="1400" b="0" i="0"/>
         </a:p>
         <a:p>
           <a:r>
             <a:rPr lang="de-CH" sz="1400" b="0" i="0"/>
-            <a:t>Average 2016-2020 = +1.3%</a:t>
+            <a:t>See electricity prices excel</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -3016,7 +3152,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="de-CH" sz="1400" b="0" i="0"/>
-            <a:t>Average 2014-2018 = -5.1%</a:t>
+            <a:t>Average 2015-2019 = -6.1%</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -3585,34 +3721,34 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BA49"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:BB49"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D58" sqref="D58"/>
+    <sheetView tabSelected="1" topLeftCell="AL1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AR54" sqref="AR54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="7.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.90625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.7265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.6328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.26953125" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="19.26953125" customWidth="1"/>
-    <col min="11" max="18" width="17.453125" bestFit="1" customWidth="1"/>
-    <col min="19" max="24" width="17.26953125" bestFit="1" customWidth="1"/>
-    <col min="25" max="32" width="17.453125" bestFit="1" customWidth="1"/>
-    <col min="33" max="38" width="17.26953125" bestFit="1" customWidth="1"/>
-    <col min="39" max="46" width="17.7265625" bestFit="1" customWidth="1"/>
-    <col min="47" max="52" width="17.54296875" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.4609375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.07421875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.69140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.921875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.69140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.84375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.61328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.23046875" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="19.23046875" customWidth="1"/>
+    <col min="11" max="18" width="17.4609375" bestFit="1" customWidth="1"/>
+    <col min="19" max="24" width="17.23046875" bestFit="1" customWidth="1"/>
+    <col min="25" max="32" width="17.4609375" bestFit="1" customWidth="1"/>
+    <col min="33" max="38" width="17.23046875" bestFit="1" customWidth="1"/>
+    <col min="39" max="46" width="17.69140625" bestFit="1" customWidth="1"/>
+    <col min="47" max="52" width="17.53515625" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="17.3828125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:53" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3686,7 +3822,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="2" spans="1:53" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:53" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
         <v>71</v>
       </c>
@@ -3696,6 +3832,9 @@
       <c r="C2" t="s">
         <v>2</v>
       </c>
+      <c r="D2" t="s">
+        <v>117</v>
+      </c>
       <c r="F2" t="s">
         <v>2</v>
       </c>
@@ -3759,13 +3898,13 @@
       <c r="Z2" s="24" t="s">
         <v>81</v>
       </c>
-      <c r="AA2" s="24" t="s">
+      <c r="AA2" s="39" t="s">
         <v>81</v>
       </c>
       <c r="AB2" s="24" t="s">
         <v>81</v>
       </c>
-      <c r="AC2" s="24" t="s">
+      <c r="AC2" s="39" t="s">
         <v>81</v>
       </c>
       <c r="AD2" s="24" t="s">
@@ -3789,7 +3928,7 @@
       <c r="AJ2" s="24" t="s">
         <v>81</v>
       </c>
-      <c r="AK2" s="24" t="s">
+      <c r="AK2" s="39" t="s">
         <v>81</v>
       </c>
       <c r="AL2" s="24" t="s">
@@ -3841,7 +3980,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="3" spans="1:53" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:53" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
         <v>44</v>
       </c>
@@ -3851,6 +3990,10 @@
       <c r="C3" t="s">
         <v>46</v>
       </c>
+      <c r="D3" s="31">
+        <f>AVERAGE(D29:D33)</f>
+        <v>-6.062113060428849E-2</v>
+      </c>
       <c r="F3" t="s">
         <v>47</v>
       </c>
@@ -3914,13 +4057,13 @@
       <c r="Z3" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="AA3" s="25" t="s">
+      <c r="AA3" s="40" t="s">
         <v>47</v>
       </c>
       <c r="AB3" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="AC3" s="25" t="s">
+      <c r="AC3" s="40" t="s">
         <v>47</v>
       </c>
       <c r="AD3" s="25" t="s">
@@ -3944,7 +4087,7 @@
       <c r="AJ3" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="AK3" s="25" t="s">
+      <c r="AK3" s="40" t="s">
         <v>47</v>
       </c>
       <c r="AL3" s="25" t="s">
@@ -3996,7 +4139,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:53" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:53" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -4075,13 +4218,13 @@
       <c r="Z4" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="AA4" s="26" t="s">
+      <c r="AA4" s="41" t="s">
         <v>40</v>
       </c>
       <c r="AB4" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="AC4" s="26" t="s">
+      <c r="AC4" s="41" t="s">
         <v>42</v>
       </c>
       <c r="AD4" s="26" t="s">
@@ -4105,7 +4248,7 @@
       <c r="AJ4" s="26" t="s">
         <v>78</v>
       </c>
-      <c r="AK4" s="26" t="s">
+      <c r="AK4" s="41" t="s">
         <v>79</v>
       </c>
       <c r="AL4" s="26" t="s">
@@ -4157,7 +4300,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="5" spans="1:53" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:53" x14ac:dyDescent="0.4">
       <c r="A5" s="1">
         <v>1991</v>
       </c>
@@ -4168,7 +4311,7 @@
         <v>13</v>
       </c>
       <c r="D5" s="22" t="e">
-        <f t="shared" ref="D5:D32" si="0">(C5-C4)/C4</f>
+        <f t="shared" ref="D5:D33" si="0">(C5-C4)/C4</f>
         <v>#VALUE!</v>
       </c>
       <c r="E5" s="22"/>
@@ -4192,9 +4335,9 @@
       <c r="M5" s="22"/>
       <c r="Y5" s="27"/>
       <c r="Z5" s="27"/>
-      <c r="AA5" s="27"/>
+      <c r="AA5" s="42"/>
       <c r="AB5" s="25"/>
-      <c r="AC5" s="25"/>
+      <c r="AC5" s="40"/>
       <c r="AD5" s="25"/>
       <c r="AE5" s="25"/>
       <c r="AF5" s="25"/>
@@ -4202,10 +4345,10 @@
       <c r="AH5" s="25"/>
       <c r="AI5" s="25"/>
       <c r="AJ5" s="25"/>
-      <c r="AK5" s="25"/>
+      <c r="AK5" s="40"/>
       <c r="AL5" s="25"/>
     </row>
-    <row r="6" spans="1:53" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:53" x14ac:dyDescent="0.4">
       <c r="A6" s="1">
         <v>1992</v>
       </c>
@@ -4240,9 +4383,9 @@
       <c r="M6" s="22"/>
       <c r="Y6" s="27"/>
       <c r="Z6" s="27"/>
-      <c r="AA6" s="27"/>
+      <c r="AA6" s="42"/>
       <c r="AB6" s="25"/>
-      <c r="AC6" s="25"/>
+      <c r="AC6" s="40"/>
       <c r="AD6" s="25"/>
       <c r="AE6" s="25"/>
       <c r="AF6" s="25"/>
@@ -4250,10 +4393,10 @@
       <c r="AH6" s="25"/>
       <c r="AI6" s="25"/>
       <c r="AJ6" s="25"/>
-      <c r="AK6" s="25"/>
+      <c r="AK6" s="40"/>
       <c r="AL6" s="25"/>
     </row>
-    <row r="7" spans="1:53" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:53" x14ac:dyDescent="0.4">
       <c r="A7" s="1">
         <v>1993</v>
       </c>
@@ -4288,9 +4431,9 @@
       <c r="M7" s="22"/>
       <c r="Y7" s="27"/>
       <c r="Z7" s="27"/>
-      <c r="AA7" s="27"/>
+      <c r="AA7" s="42"/>
       <c r="AB7" s="25"/>
-      <c r="AC7" s="25"/>
+      <c r="AC7" s="40"/>
       <c r="AD7" s="25"/>
       <c r="AE7" s="25"/>
       <c r="AF7" s="25"/>
@@ -4298,10 +4441,10 @@
       <c r="AH7" s="25"/>
       <c r="AI7" s="25"/>
       <c r="AJ7" s="25"/>
-      <c r="AK7" s="25"/>
+      <c r="AK7" s="40"/>
       <c r="AL7" s="25"/>
     </row>
-    <row r="8" spans="1:53" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:53" x14ac:dyDescent="0.4">
       <c r="A8" s="1">
         <v>1994</v>
       </c>
@@ -4336,9 +4479,9 @@
       <c r="M8" s="22"/>
       <c r="Y8" s="27"/>
       <c r="Z8" s="27"/>
-      <c r="AA8" s="27"/>
+      <c r="AA8" s="42"/>
       <c r="AB8" s="25"/>
-      <c r="AC8" s="25"/>
+      <c r="AC8" s="40"/>
       <c r="AD8" s="25"/>
       <c r="AE8" s="25"/>
       <c r="AF8" s="25"/>
@@ -4346,10 +4489,10 @@
       <c r="AH8" s="25"/>
       <c r="AI8" s="25"/>
       <c r="AJ8" s="25"/>
-      <c r="AK8" s="25"/>
+      <c r="AK8" s="40"/>
       <c r="AL8" s="25"/>
     </row>
-    <row r="9" spans="1:53" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:53" x14ac:dyDescent="0.4">
       <c r="A9" s="1">
         <v>1995</v>
       </c>
@@ -4384,9 +4527,9 @@
       <c r="M9" s="22"/>
       <c r="Y9" s="27"/>
       <c r="Z9" s="27"/>
-      <c r="AA9" s="27"/>
+      <c r="AA9" s="42"/>
       <c r="AB9" s="25"/>
-      <c r="AC9" s="25"/>
+      <c r="AC9" s="40"/>
       <c r="AD9" s="25"/>
       <c r="AE9" s="25"/>
       <c r="AF9" s="25"/>
@@ -4394,10 +4537,10 @@
       <c r="AH9" s="25"/>
       <c r="AI9" s="25"/>
       <c r="AJ9" s="25"/>
-      <c r="AK9" s="25"/>
+      <c r="AK9" s="40"/>
       <c r="AL9" s="25"/>
     </row>
-    <row r="10" spans="1:53" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:53" x14ac:dyDescent="0.4">
       <c r="A10" s="1">
         <v>1996</v>
       </c>
@@ -4432,9 +4575,9 @@
       <c r="M10" s="22"/>
       <c r="Y10" s="27"/>
       <c r="Z10" s="27"/>
-      <c r="AA10" s="27"/>
+      <c r="AA10" s="42"/>
       <c r="AB10" s="25"/>
-      <c r="AC10" s="25"/>
+      <c r="AC10" s="40"/>
       <c r="AD10" s="25"/>
       <c r="AE10" s="25"/>
       <c r="AF10" s="25"/>
@@ -4442,10 +4585,10 @@
       <c r="AH10" s="25"/>
       <c r="AI10" s="25"/>
       <c r="AJ10" s="25"/>
-      <c r="AK10" s="25"/>
+      <c r="AK10" s="40"/>
       <c r="AL10" s="25"/>
     </row>
-    <row r="11" spans="1:53" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:53" x14ac:dyDescent="0.4">
       <c r="A11" s="1">
         <v>1997</v>
       </c>
@@ -4480,9 +4623,9 @@
       <c r="M11" s="22"/>
       <c r="Y11" s="27"/>
       <c r="Z11" s="27"/>
-      <c r="AA11" s="27"/>
+      <c r="AA11" s="42"/>
       <c r="AB11" s="25"/>
-      <c r="AC11" s="25"/>
+      <c r="AC11" s="40"/>
       <c r="AD11" s="25"/>
       <c r="AE11" s="25"/>
       <c r="AF11" s="25"/>
@@ -4490,10 +4633,10 @@
       <c r="AH11" s="25"/>
       <c r="AI11" s="25"/>
       <c r="AJ11" s="25"/>
-      <c r="AK11" s="25"/>
+      <c r="AK11" s="40"/>
       <c r="AL11" s="25"/>
     </row>
-    <row r="12" spans="1:53" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:53" x14ac:dyDescent="0.4">
       <c r="A12" s="1">
         <v>1998</v>
       </c>
@@ -4528,9 +4671,9 @@
       <c r="M12" s="22"/>
       <c r="Y12" s="27"/>
       <c r="Z12" s="27"/>
-      <c r="AA12" s="27"/>
+      <c r="AA12" s="42"/>
       <c r="AB12" s="25"/>
-      <c r="AC12" s="25"/>
+      <c r="AC12" s="40"/>
       <c r="AD12" s="25"/>
       <c r="AE12" s="25"/>
       <c r="AF12" s="25"/>
@@ -4538,10 +4681,10 @@
       <c r="AH12" s="25"/>
       <c r="AI12" s="25"/>
       <c r="AJ12" s="25"/>
-      <c r="AK12" s="25"/>
+      <c r="AK12" s="40"/>
       <c r="AL12" s="25"/>
     </row>
-    <row r="13" spans="1:53" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:53" x14ac:dyDescent="0.4">
       <c r="A13" s="1">
         <v>1999</v>
       </c>
@@ -4576,9 +4719,9 @@
       <c r="M13" s="22"/>
       <c r="Y13" s="27"/>
       <c r="Z13" s="27"/>
-      <c r="AA13" s="27"/>
+      <c r="AA13" s="42"/>
       <c r="AB13" s="25"/>
-      <c r="AC13" s="25"/>
+      <c r="AC13" s="40"/>
       <c r="AD13" s="25"/>
       <c r="AE13" s="25"/>
       <c r="AF13" s="25"/>
@@ -4586,10 +4729,10 @@
       <c r="AH13" s="25"/>
       <c r="AI13" s="25"/>
       <c r="AJ13" s="25"/>
-      <c r="AK13" s="25"/>
+      <c r="AK13" s="40"/>
       <c r="AL13" s="25"/>
     </row>
-    <row r="14" spans="1:53" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:53" x14ac:dyDescent="0.4">
       <c r="A14" s="1">
         <v>2000</v>
       </c>
@@ -4624,9 +4767,9 @@
       <c r="M14" s="22"/>
       <c r="Y14" s="27"/>
       <c r="Z14" s="27"/>
-      <c r="AA14" s="27"/>
+      <c r="AA14" s="42"/>
       <c r="AB14" s="25"/>
-      <c r="AC14" s="25"/>
+      <c r="AC14" s="40"/>
       <c r="AD14" s="25"/>
       <c r="AE14" s="25"/>
       <c r="AF14" s="25"/>
@@ -4634,10 +4777,10 @@
       <c r="AH14" s="25"/>
       <c r="AI14" s="25"/>
       <c r="AJ14" s="25"/>
-      <c r="AK14" s="25"/>
+      <c r="AK14" s="40"/>
       <c r="AL14" s="25"/>
     </row>
-    <row r="15" spans="1:53" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:53" x14ac:dyDescent="0.4">
       <c r="A15" s="1">
         <v>2001</v>
       </c>
@@ -4672,9 +4815,9 @@
       <c r="M15" s="22"/>
       <c r="Y15" s="27"/>
       <c r="Z15" s="27"/>
-      <c r="AA15" s="27"/>
+      <c r="AA15" s="42"/>
       <c r="AB15" s="25"/>
-      <c r="AC15" s="25"/>
+      <c r="AC15" s="40"/>
       <c r="AD15" s="25"/>
       <c r="AE15" s="25"/>
       <c r="AF15" s="25"/>
@@ -4682,10 +4825,10 @@
       <c r="AH15" s="25"/>
       <c r="AI15" s="25"/>
       <c r="AJ15" s="25"/>
-      <c r="AK15" s="25"/>
+      <c r="AK15" s="40"/>
       <c r="AL15" s="25"/>
     </row>
-    <row r="16" spans="1:53" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:53" x14ac:dyDescent="0.4">
       <c r="A16" s="1">
         <v>2002</v>
       </c>
@@ -4720,9 +4863,9 @@
       <c r="M16" s="22"/>
       <c r="Y16" s="27"/>
       <c r="Z16" s="27"/>
-      <c r="AA16" s="27"/>
+      <c r="AA16" s="42"/>
       <c r="AB16" s="25"/>
-      <c r="AC16" s="25"/>
+      <c r="AC16" s="40"/>
       <c r="AD16" s="25"/>
       <c r="AE16" s="25"/>
       <c r="AF16" s="25"/>
@@ -4730,10 +4873,10 @@
       <c r="AH16" s="25"/>
       <c r="AI16" s="25"/>
       <c r="AJ16" s="25"/>
-      <c r="AK16" s="25"/>
+      <c r="AK16" s="40"/>
       <c r="AL16" s="25"/>
     </row>
-    <row r="17" spans="1:53" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:53" x14ac:dyDescent="0.4">
       <c r="A17" s="1">
         <v>2003</v>
       </c>
@@ -4768,9 +4911,9 @@
       <c r="M17" s="22"/>
       <c r="Y17" s="27"/>
       <c r="Z17" s="27"/>
-      <c r="AA17" s="27"/>
+      <c r="AA17" s="42"/>
       <c r="AB17" s="25"/>
-      <c r="AC17" s="25"/>
+      <c r="AC17" s="40"/>
       <c r="AD17" s="25"/>
       <c r="AE17" s="25"/>
       <c r="AF17" s="25"/>
@@ -4778,10 +4921,10 @@
       <c r="AH17" s="25"/>
       <c r="AI17" s="25"/>
       <c r="AJ17" s="25"/>
-      <c r="AK17" s="25"/>
+      <c r="AK17" s="40"/>
       <c r="AL17" s="25"/>
     </row>
-    <row r="18" spans="1:53" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:53" x14ac:dyDescent="0.4">
       <c r="A18" s="1">
         <v>2004</v>
       </c>
@@ -4816,9 +4959,9 @@
       <c r="M18" s="22"/>
       <c r="Y18" s="27"/>
       <c r="Z18" s="27"/>
-      <c r="AA18" s="27"/>
+      <c r="AA18" s="42"/>
       <c r="AB18" s="25"/>
-      <c r="AC18" s="25"/>
+      <c r="AC18" s="40"/>
       <c r="AD18" s="25"/>
       <c r="AE18" s="25"/>
       <c r="AF18" s="25"/>
@@ -4826,10 +4969,10 @@
       <c r="AH18" s="25"/>
       <c r="AI18" s="25"/>
       <c r="AJ18" s="25"/>
-      <c r="AK18" s="25"/>
+      <c r="AK18" s="40"/>
       <c r="AL18" s="25"/>
     </row>
-    <row r="19" spans="1:53" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:53" x14ac:dyDescent="0.4">
       <c r="A19" s="1">
         <v>2005</v>
       </c>
@@ -4864,9 +5007,9 @@
       <c r="M19" s="22"/>
       <c r="Y19" s="27"/>
       <c r="Z19" s="27"/>
-      <c r="AA19" s="27"/>
+      <c r="AA19" s="42"/>
       <c r="AB19" s="25"/>
-      <c r="AC19" s="25"/>
+      <c r="AC19" s="40"/>
       <c r="AD19" s="25"/>
       <c r="AE19" s="25"/>
       <c r="AF19" s="25"/>
@@ -4874,10 +5017,10 @@
       <c r="AH19" s="25"/>
       <c r="AI19" s="25"/>
       <c r="AJ19" s="25"/>
-      <c r="AK19" s="25"/>
+      <c r="AK19" s="40"/>
       <c r="AL19" s="25"/>
     </row>
-    <row r="20" spans="1:53" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:53" x14ac:dyDescent="0.4">
       <c r="A20" s="1">
         <v>2006</v>
       </c>
@@ -4912,9 +5055,9 @@
       <c r="M20" s="22"/>
       <c r="Y20" s="27"/>
       <c r="Z20" s="27"/>
-      <c r="AA20" s="27"/>
+      <c r="AA20" s="42"/>
       <c r="AB20" s="25"/>
-      <c r="AC20" s="25"/>
+      <c r="AC20" s="40"/>
       <c r="AD20" s="25"/>
       <c r="AE20" s="25"/>
       <c r="AF20" s="25"/>
@@ -4922,10 +5065,10 @@
       <c r="AH20" s="25"/>
       <c r="AI20" s="25"/>
       <c r="AJ20" s="25"/>
-      <c r="AK20" s="25"/>
+      <c r="AK20" s="40"/>
       <c r="AL20" s="25"/>
     </row>
-    <row r="21" spans="1:53" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:53" x14ac:dyDescent="0.4">
       <c r="A21" s="1">
         <v>2007</v>
       </c>
@@ -4960,9 +5103,9 @@
       <c r="M21" s="22"/>
       <c r="Y21" s="27"/>
       <c r="Z21" s="27"/>
-      <c r="AA21" s="27"/>
+      <c r="AA21" s="42"/>
       <c r="AB21" s="25"/>
-      <c r="AC21" s="25"/>
+      <c r="AC21" s="40"/>
       <c r="AD21" s="25"/>
       <c r="AE21" s="25"/>
       <c r="AF21" s="25"/>
@@ -4970,10 +5113,10 @@
       <c r="AH21" s="25"/>
       <c r="AI21" s="25"/>
       <c r="AJ21" s="25"/>
-      <c r="AK21" s="25"/>
+      <c r="AK21" s="40"/>
       <c r="AL21" s="25"/>
     </row>
-    <row r="22" spans="1:53" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:53" x14ac:dyDescent="0.4">
       <c r="A22" s="1">
         <v>2008</v>
       </c>
@@ -5008,9 +5151,9 @@
       <c r="M22" s="22"/>
       <c r="Y22" s="27"/>
       <c r="Z22" s="27"/>
-      <c r="AA22" s="27"/>
+      <c r="AA22" s="42"/>
       <c r="AB22" s="25"/>
-      <c r="AC22" s="25"/>
+      <c r="AC22" s="40"/>
       <c r="AD22" s="25"/>
       <c r="AE22" s="25"/>
       <c r="AF22" s="25"/>
@@ -5018,10 +5161,10 @@
       <c r="AH22" s="25"/>
       <c r="AI22" s="25"/>
       <c r="AJ22" s="25"/>
-      <c r="AK22" s="25"/>
+      <c r="AK22" s="40"/>
       <c r="AL22" s="25"/>
     </row>
-    <row r="23" spans="1:53" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:53" x14ac:dyDescent="0.4">
       <c r="A23" s="1">
         <v>2009</v>
       </c>
@@ -5099,7 +5242,7 @@
         <f t="shared" ref="Z23:AL23" si="1">L23*1.077</f>
         <v>13.945180628571396</v>
       </c>
-      <c r="AA23" s="28">
+      <c r="AA23" s="43">
         <f t="shared" si="1"/>
         <v>11.409122571428602</v>
       </c>
@@ -5107,7 +5250,7 @@
         <f t="shared" si="1"/>
         <v>13.825910571428601</v>
       </c>
-      <c r="AC23" s="28">
+      <c r="AC23" s="43">
         <f t="shared" si="1"/>
         <v>11.6476626857143</v>
       </c>
@@ -5139,7 +5282,7 @@
         <f t="shared" si="1"/>
         <v>14.76895485</v>
       </c>
-      <c r="AK23" s="28"/>
+      <c r="AK23" s="43"/>
       <c r="AL23" s="28">
         <f t="shared" si="1"/>
         <v>10.388235462194061</v>
@@ -5192,12 +5335,8 @@
         <f t="shared" ref="AX23:AX34" si="13">(V23-V22)/V22</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AY23" t="e">
-        <f t="shared" ref="AY23:AY34" si="14">(W23-W22)/W22</f>
-        <v>#DIV/0!</v>
-      </c>
       <c r="AZ23" t="e">
-        <f t="shared" ref="AZ23:AZ34" si="15">(X23-X22)/X22</f>
+        <f t="shared" ref="AZ23:AZ34" si="14">(X23-X22)/X22</f>
         <v>#DIV/0!</v>
       </c>
       <c r="BA23" t="e">
@@ -5205,7 +5344,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="24" spans="1:53" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:53" x14ac:dyDescent="0.4">
       <c r="A24" s="1">
         <v>2010</v>
       </c>
@@ -5276,56 +5415,56 @@
         <v>9.6455296770604093</v>
       </c>
       <c r="Y24" s="28">
-        <f t="shared" ref="Y24:Y34" si="16">K24*1.077</f>
+        <f t="shared" ref="Y24:Y34" si="15">K24*1.077</f>
         <v>14.241786428571398</v>
       </c>
       <c r="Z24" s="28">
-        <f t="shared" ref="Z24:Z34" si="17">L24*1.077</f>
+        <f t="shared" ref="Z24:Z34" si="16">L24*1.077</f>
         <v>13.945180628571396</v>
       </c>
-      <c r="AA24" s="28">
-        <f t="shared" ref="AA24:AA34" si="18">M24*1.077</f>
+      <c r="AA24" s="43">
+        <f t="shared" ref="AA24:AA34" si="17">M24*1.077</f>
         <v>11.409122571428602</v>
       </c>
       <c r="AB24" s="28">
-        <f t="shared" ref="AB24:AB34" si="19">N24*1.077</f>
+        <f t="shared" ref="AB24:AB34" si="18">N24*1.077</f>
         <v>13.825910571428601</v>
       </c>
-      <c r="AC24" s="28">
-        <f t="shared" ref="AC24:AC34" si="20">O24*1.077</f>
+      <c r="AC24" s="43">
+        <f t="shared" ref="AC24:AC34" si="19">O24*1.077</f>
         <v>11.6476626857143</v>
       </c>
       <c r="AD24" s="28">
-        <f t="shared" ref="AD24:AD34" si="21">P24*1.077</f>
+        <f t="shared" ref="AD24:AD34" si="20">P24*1.077</f>
         <v>9.2616338057142897</v>
       </c>
       <c r="AE24" s="28">
-        <f t="shared" ref="AE24:AE34" si="22">Q24*1.077</f>
+        <f t="shared" ref="AE24:AE34" si="21">Q24*1.077</f>
         <v>11.297115754945088</v>
       </c>
       <c r="AF24" s="28">
-        <f t="shared" ref="AF24:AF34" si="23">R24*1.077</f>
+        <f t="shared" ref="AF24:AF34" si="22">R24*1.077</f>
         <v>13.827479914285698</v>
       </c>
       <c r="AG24" s="28">
-        <f t="shared" ref="AG24:AG34" si="24">S24*1.077</f>
+        <f t="shared" ref="AG24:AG34" si="23">S24*1.077</f>
         <v>15.4791151875</v>
       </c>
       <c r="AH24" s="28">
-        <f t="shared" ref="AH24:AH34" si="25">T24*1.077</f>
+        <f t="shared" ref="AH24:AH34" si="24">T24*1.077</f>
         <v>15.349350149999999</v>
       </c>
       <c r="AI24" s="28">
-        <f t="shared" ref="AI24:AI34" si="26">U24*1.077</f>
+        <f t="shared" ref="AI24:AI34" si="25">U24*1.077</f>
         <v>16.096662499999965</v>
       </c>
       <c r="AJ24" s="28">
-        <f t="shared" ref="AJ24:AJ34" si="27">V24*1.077</f>
+        <f t="shared" ref="AJ24:AJ34" si="26">V24*1.077</f>
         <v>14.76895485</v>
       </c>
-      <c r="AK24" s="28"/>
+      <c r="AK24" s="43"/>
       <c r="AL24" s="28">
-        <f t="shared" ref="AL24:AL34" si="28">X24*1.077</f>
+        <f t="shared" ref="AL24:AL34" si="27">X24*1.077</f>
         <v>10.388235462194061</v>
       </c>
       <c r="AM24">
@@ -5376,20 +5515,16 @@
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="AY24" t="e">
+      <c r="AZ24">
         <f t="shared" si="14"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AZ24">
-        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="BA24">
-        <f t="shared" ref="BA24:BA34" si="29">_xlfn.AGGREGATE(1,3,AM24:AZ24)</f>
+        <f t="shared" ref="BA24:BA34" si="28">_xlfn.AGGREGATE(1,3,AM24:AZ24)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:53" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:53" x14ac:dyDescent="0.4">
       <c r="A25" s="1">
         <v>2011</v>
       </c>
@@ -5460,56 +5595,56 @@
         <v>9.6455296770604093</v>
       </c>
       <c r="Y25" s="28">
+        <f t="shared" si="15"/>
+        <v>14.241786428571398</v>
+      </c>
+      <c r="Z25" s="28">
         <f t="shared" si="16"/>
-        <v>14.241786428571398</v>
-      </c>
-      <c r="Z25" s="28">
+        <v>13.945180628571396</v>
+      </c>
+      <c r="AA25" s="43">
         <f t="shared" si="17"/>
-        <v>13.945180628571396</v>
-      </c>
-      <c r="AA25" s="28">
+        <v>11.409122571428602</v>
+      </c>
+      <c r="AB25" s="28">
         <f t="shared" si="18"/>
-        <v>11.409122571428602</v>
-      </c>
-      <c r="AB25" s="28">
+        <v>13.825910571428601</v>
+      </c>
+      <c r="AC25" s="43">
         <f t="shared" si="19"/>
-        <v>13.825910571428601</v>
-      </c>
-      <c r="AC25" s="28">
+        <v>11.6476626857143</v>
+      </c>
+      <c r="AD25" s="28">
         <f t="shared" si="20"/>
-        <v>11.6476626857143</v>
-      </c>
-      <c r="AD25" s="28">
+        <v>9.2616338057142897</v>
+      </c>
+      <c r="AE25" s="28">
         <f t="shared" si="21"/>
-        <v>9.2616338057142897</v>
-      </c>
-      <c r="AE25" s="28">
+        <v>11.297115754945088</v>
+      </c>
+      <c r="AF25" s="28">
         <f t="shared" si="22"/>
-        <v>11.297115754945088</v>
-      </c>
-      <c r="AF25" s="28">
+        <v>13.827479914285698</v>
+      </c>
+      <c r="AG25" s="28">
         <f t="shared" si="23"/>
-        <v>13.827479914285698</v>
-      </c>
-      <c r="AG25" s="28">
+        <v>15.4791151875</v>
+      </c>
+      <c r="AH25" s="28">
         <f t="shared" si="24"/>
-        <v>15.4791151875</v>
-      </c>
-      <c r="AH25" s="28">
+        <v>15.349350149999999</v>
+      </c>
+      <c r="AI25" s="28">
         <f t="shared" si="25"/>
-        <v>15.349350149999999</v>
-      </c>
-      <c r="AI25" s="28">
+        <v>16.096662499999965</v>
+      </c>
+      <c r="AJ25" s="28">
         <f t="shared" si="26"/>
-        <v>16.096662499999965</v>
-      </c>
-      <c r="AJ25" s="28">
+        <v>14.76895485</v>
+      </c>
+      <c r="AK25" s="43"/>
+      <c r="AL25" s="28">
         <f t="shared" si="27"/>
-        <v>14.76895485</v>
-      </c>
-      <c r="AK25" s="28"/>
-      <c r="AL25" s="28">
-        <f t="shared" si="28"/>
         <v>10.388235462194061</v>
       </c>
       <c r="AM25">
@@ -5560,20 +5695,16 @@
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="AY25" t="e">
+      <c r="AZ25">
         <f t="shared" si="14"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AZ25">
-        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="BA25">
-        <f t="shared" si="29"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:53" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:53" x14ac:dyDescent="0.4">
       <c r="A26" s="1">
         <v>2012</v>
       </c>
@@ -5644,56 +5775,56 @@
         <v>10.4978162045785</v>
       </c>
       <c r="Y26" s="28">
+        <f t="shared" si="15"/>
+        <v>15.498991607142903</v>
+      </c>
+      <c r="Z26" s="28">
         <f t="shared" si="16"/>
-        <v>15.498991607142903</v>
-      </c>
-      <c r="Z26" s="28">
+        <v>15.172606757142903</v>
+      </c>
+      <c r="AA26" s="43">
         <f t="shared" si="17"/>
-        <v>15.172606757142903</v>
-      </c>
-      <c r="AA26" s="28">
+        <v>12.415322642857168</v>
+      </c>
+      <c r="AB26" s="28">
         <f t="shared" si="18"/>
-        <v>12.415322642857168</v>
-      </c>
-      <c r="AB26" s="28">
+        <v>15.050023642857132</v>
+      </c>
+      <c r="AC26" s="43">
         <f t="shared" si="19"/>
-        <v>15.050023642857132</v>
-      </c>
-      <c r="AC26" s="28">
+        <v>12.671258871428602</v>
+      </c>
+      <c r="AD26" s="28">
         <f t="shared" si="20"/>
-        <v>12.671258871428602</v>
-      </c>
-      <c r="AD26" s="28">
+        <v>10.07894141142857</v>
+      </c>
+      <c r="AE26" s="28">
         <f t="shared" si="21"/>
-        <v>10.07894141142857</v>
-      </c>
-      <c r="AE26" s="28">
+        <v>12.29038728956048</v>
+      </c>
+      <c r="AF26" s="28">
         <f t="shared" si="22"/>
-        <v>12.29038728956048</v>
-      </c>
-      <c r="AF26" s="28">
+        <v>15.051636578571397</v>
+      </c>
+      <c r="AG26" s="28">
         <f t="shared" si="23"/>
-        <v>15.051636578571397</v>
-      </c>
-      <c r="AG26" s="28">
+        <v>16.846080609375001</v>
+      </c>
+      <c r="AH26" s="28">
         <f t="shared" si="24"/>
-        <v>16.846080609375001</v>
-      </c>
-      <c r="AH26" s="28">
+        <v>16.701940987499999</v>
+      </c>
+      <c r="AI26" s="28">
         <f t="shared" si="25"/>
-        <v>16.701940987499999</v>
-      </c>
-      <c r="AI26" s="28">
+        <v>17.515834375000036</v>
+      </c>
+      <c r="AJ26" s="28">
         <f t="shared" si="26"/>
-        <v>17.515834375000036</v>
-      </c>
-      <c r="AJ26" s="28">
+        <v>16.0674802875</v>
+      </c>
+      <c r="AK26" s="43"/>
+      <c r="AL26" s="28">
         <f t="shared" si="27"/>
-        <v>16.0674802875</v>
-      </c>
-      <c r="AK26" s="28"/>
-      <c r="AL26" s="28">
-        <f t="shared" si="28"/>
         <v>11.306148052331045</v>
       </c>
       <c r="AM26">
@@ -5744,20 +5875,16 @@
         <f t="shared" si="13"/>
         <v>8.7922635737490915E-2</v>
       </c>
-      <c r="AY26" t="e">
+      <c r="AZ26">
         <f t="shared" si="14"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AZ26">
-        <f t="shared" si="15"/>
         <v>8.8360780180382528E-2</v>
       </c>
       <c r="BA26">
-        <f t="shared" si="29"/>
+        <f t="shared" si="28"/>
         <v>8.8191039627855516E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:53" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:53" x14ac:dyDescent="0.4">
       <c r="A27" s="1">
         <v>2013</v>
       </c>
@@ -5828,56 +5955,56 @@
         <v>12.6022669065544</v>
       </c>
       <c r="Y27" s="28">
+        <f t="shared" si="15"/>
+        <v>17.707033928571398</v>
+      </c>
+      <c r="Z27" s="28">
         <f t="shared" si="16"/>
-        <v>17.707033928571398</v>
-      </c>
-      <c r="Z27" s="28">
+        <v>17.349362228571398</v>
+      </c>
+      <c r="AA27" s="43">
         <f t="shared" si="17"/>
-        <v>17.349362228571398</v>
-      </c>
-      <c r="AA27" s="28">
+        <v>14.291174571428602</v>
+      </c>
+      <c r="AB27" s="28">
         <f t="shared" si="18"/>
-        <v>14.291174571428602</v>
-      </c>
-      <c r="AB27" s="28">
+        <v>17.205536571428603</v>
+      </c>
+      <c r="AC27" s="43">
         <f t="shared" si="19"/>
-        <v>17.205536571428603</v>
-      </c>
-      <c r="AC27" s="28">
+        <v>14.578825885714302</v>
+      </c>
+      <c r="AD27" s="28">
         <f t="shared" si="20"/>
-        <v>14.578825885714302</v>
-      </c>
-      <c r="AD27" s="28">
+        <v>11.7015557657143</v>
+      </c>
+      <c r="AE27" s="28">
         <f t="shared" si="21"/>
-        <v>11.7015557657143</v>
-      </c>
-      <c r="AE27" s="28">
+        <v>15.043983369230784</v>
+      </c>
+      <c r="AF27" s="28">
         <f t="shared" si="22"/>
-        <v>15.043983369230784</v>
-      </c>
-      <c r="AF27" s="28">
+        <v>17.207429014285697</v>
+      </c>
+      <c r="AG27" s="28">
         <f t="shared" si="23"/>
-        <v>17.207429014285697</v>
-      </c>
-      <c r="AG27" s="28">
+        <v>19.199106843749998</v>
+      </c>
+      <c r="AH27" s="28">
         <f t="shared" si="24"/>
-        <v>19.199106843749998</v>
-      </c>
-      <c r="AH27" s="28">
+        <v>19.042625474999998</v>
+      </c>
+      <c r="AI27" s="28">
         <f t="shared" si="25"/>
-        <v>19.042625474999998</v>
-      </c>
-      <c r="AI27" s="28">
+        <v>18.695373749999998</v>
+      </c>
+      <c r="AJ27" s="28">
         <f t="shared" si="26"/>
-        <v>18.695373749999998</v>
-      </c>
-      <c r="AJ27" s="28">
+        <v>16.429392674999999</v>
+      </c>
+      <c r="AK27" s="43"/>
+      <c r="AL27" s="28">
         <f t="shared" si="27"/>
-        <v>16.429392674999999</v>
-      </c>
-      <c r="AK27" s="28"/>
-      <c r="AL27" s="28">
-        <f t="shared" si="28"/>
         <v>13.572641458359088</v>
       </c>
       <c r="AM27">
@@ -5928,20 +6055,16 @@
         <f t="shared" si="13"/>
         <v>2.2524526622979976E-2</v>
       </c>
-      <c r="AY27" t="e">
+      <c r="AZ27">
         <f t="shared" si="14"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AZ27">
-        <f t="shared" si="15"/>
         <v>0.20046556931126952</v>
       </c>
       <c r="BA27">
-        <f t="shared" si="29"/>
+        <f t="shared" si="28"/>
         <v>0.14070792426841286</v>
       </c>
     </row>
-    <row r="28" spans="1:53" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:53" x14ac:dyDescent="0.4">
       <c r="A28" s="1">
         <v>2014</v>
       </c>
@@ -6013,56 +6136,56 @@
         <v>13.966288029918299</v>
       </c>
       <c r="Y28" s="28">
+        <f t="shared" si="15"/>
+        <v>17.849890285714299</v>
+      </c>
+      <c r="Z28" s="28">
         <f t="shared" si="16"/>
-        <v>17.849890285714299</v>
-      </c>
-      <c r="Z28" s="28">
+        <v>17.4895691657143</v>
+      </c>
+      <c r="AA28" s="43">
         <f t="shared" si="17"/>
-        <v>17.4895691657143</v>
-      </c>
-      <c r="AA28" s="28">
+        <v>14.4372773142857</v>
+      </c>
+      <c r="AB28" s="28">
         <f t="shared" si="18"/>
-        <v>14.4372773142857</v>
-      </c>
-      <c r="AB28" s="28">
+        <v>17.346900514285696</v>
+      </c>
+      <c r="AC28" s="43">
         <f t="shared" si="19"/>
-        <v>17.346900514285696</v>
-      </c>
-      <c r="AC28" s="28">
+        <v>14.722614617142902</v>
+      </c>
+      <c r="AD28" s="28">
         <f t="shared" si="20"/>
-        <v>14.722614617142902</v>
-      </c>
-      <c r="AD28" s="28">
+        <v>11.847007385142902</v>
+      </c>
+      <c r="AE28" s="28">
         <f t="shared" si="21"/>
-        <v>11.847007385142902</v>
-      </c>
-      <c r="AE28" s="28">
+        <v>15.189181905494539</v>
+      </c>
+      <c r="AF28" s="28">
         <f t="shared" si="22"/>
-        <v>15.189181905494539</v>
-      </c>
-      <c r="AF28" s="28">
+        <v>17.348636022857097</v>
+      </c>
+      <c r="AG28" s="28">
         <f t="shared" si="23"/>
-        <v>17.348636022857097</v>
-      </c>
-      <c r="AG28" s="28">
+        <v>19.347470325</v>
+      </c>
+      <c r="AH28" s="28">
         <f t="shared" si="24"/>
-        <v>19.347470325</v>
-      </c>
-      <c r="AH28" s="28">
+        <v>19.193195459999998</v>
+      </c>
+      <c r="AI28" s="28">
         <f t="shared" si="25"/>
-        <v>19.193195459999998</v>
-      </c>
-      <c r="AI28" s="28">
+        <v>20.345606999999998</v>
+      </c>
+      <c r="AJ28" s="28">
         <f t="shared" si="26"/>
-        <v>20.345606999999998</v>
-      </c>
-      <c r="AJ28" s="28">
+        <v>18.07393398</v>
+      </c>
+      <c r="AK28" s="43"/>
+      <c r="AL28" s="28">
         <f t="shared" si="27"/>
-        <v>18.07393398</v>
-      </c>
-      <c r="AK28" s="28"/>
-      <c r="AL28" s="28">
-        <f t="shared" si="28"/>
         <v>15.041692208222008</v>
       </c>
       <c r="AM28">
@@ -6113,20 +6236,16 @@
         <f t="shared" si="13"/>
         <v>0.10009751045164539</v>
       </c>
-      <c r="AY28" t="e">
+      <c r="AZ28">
         <f t="shared" si="14"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AZ28">
-        <f t="shared" si="15"/>
         <v>0.10823617159341996</v>
       </c>
       <c r="BA28">
-        <f t="shared" si="29"/>
+        <f t="shared" si="28"/>
         <v>2.9767482187529257E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:53" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:53" x14ac:dyDescent="0.4">
       <c r="A29" s="1">
         <v>2015</v>
       </c>
@@ -6198,56 +6317,56 @@
         <v>16.314764477687</v>
       </c>
       <c r="Y29" s="28">
+        <f t="shared" si="15"/>
+        <v>21.629237142857097</v>
+      </c>
+      <c r="Z29" s="28">
         <f t="shared" si="16"/>
-        <v>21.629237142857097</v>
-      </c>
-      <c r="Z29" s="28">
+        <v>21.213084342857094</v>
+      </c>
+      <c r="AA29" s="43">
         <f t="shared" si="17"/>
-        <v>21.213084342857094</v>
-      </c>
-      <c r="AA29" s="28">
+        <v>17.651106857142903</v>
+      </c>
+      <c r="AB29" s="28">
         <f t="shared" si="18"/>
-        <v>17.651106857142903</v>
-      </c>
-      <c r="AB29" s="28">
+        <v>21.047964857142901</v>
+      </c>
+      <c r="AC29" s="43">
         <f t="shared" si="19"/>
-        <v>21.047964857142901</v>
-      </c>
-      <c r="AC29" s="28">
+        <v>17.986761600000001</v>
+      </c>
+      <c r="AD29" s="28">
         <f t="shared" si="20"/>
-        <v>17.986761600000001</v>
-      </c>
-      <c r="AD29" s="28">
+        <v>14.636688479999998</v>
+      </c>
+      <c r="AE29" s="28">
         <f t="shared" si="21"/>
-        <v>14.636688479999998</v>
-      </c>
-      <c r="AE29" s="28">
+        <v>18.083161384615391</v>
+      </c>
+      <c r="AF29" s="28">
         <f t="shared" si="22"/>
-        <v>18.083161384615391</v>
-      </c>
-      <c r="AF29" s="28">
+        <v>21.049995771428602</v>
+      </c>
+      <c r="AG29" s="28">
         <f t="shared" si="23"/>
-        <v>21.049995771428602</v>
-      </c>
-      <c r="AG29" s="28">
+        <v>23.370496124999999</v>
+      </c>
+      <c r="AH29" s="28">
         <f t="shared" si="24"/>
-        <v>23.370496124999999</v>
-      </c>
-      <c r="AH29" s="28">
+        <v>23.181024900000001</v>
+      </c>
+      <c r="AI29" s="28">
         <f t="shared" si="25"/>
-        <v>23.181024900000001</v>
-      </c>
-      <c r="AI29" s="28">
+        <v>23.670664999999964</v>
+      </c>
+      <c r="AJ29" s="28">
         <f t="shared" si="26"/>
-        <v>23.670664999999964</v>
-      </c>
-      <c r="AJ29" s="28">
+        <v>21.320722799999999</v>
+      </c>
+      <c r="AK29" s="43"/>
+      <c r="AL29" s="28">
         <f t="shared" si="27"/>
-        <v>21.320722799999999</v>
-      </c>
-      <c r="AK29" s="28"/>
-      <c r="AL29" s="28">
-        <f t="shared" si="28"/>
         <v>17.571001342468897</v>
       </c>
       <c r="AM29">
@@ -6298,20 +6417,16 @@
         <f t="shared" si="13"/>
         <v>0.17963929842793414</v>
       </c>
-      <c r="AY29" t="e">
+      <c r="AZ29">
         <f t="shared" si="14"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AZ29">
-        <f t="shared" si="15"/>
         <v>0.16815323031702062</v>
       </c>
       <c r="BA29">
-        <f t="shared" si="29"/>
+        <f t="shared" si="28"/>
         <v>0.20373744217920156</v>
       </c>
     </row>
-    <row r="30" spans="1:53" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:53" x14ac:dyDescent="0.4">
       <c r="A30" s="1">
         <v>2016</v>
       </c>
@@ -6383,56 +6498,56 @@
         <v>16.514764477686999</v>
       </c>
       <c r="Y30" s="28">
+        <f t="shared" si="15"/>
+        <v>23.147807142857097</v>
+      </c>
+      <c r="Z30" s="28">
         <f t="shared" si="16"/>
-        <v>23.147807142857097</v>
-      </c>
-      <c r="Z30" s="28">
+        <v>22.704513942857098</v>
+      </c>
+      <c r="AA30" s="43">
         <f t="shared" si="17"/>
-        <v>22.704513942857098</v>
-      </c>
-      <c r="AA30" s="28">
+        <v>18.910478857142866</v>
+      </c>
+      <c r="AB30" s="28">
         <f t="shared" si="18"/>
-        <v>18.910478857142866</v>
-      </c>
-      <c r="AB30" s="28">
+        <v>22.528480857142828</v>
+      </c>
+      <c r="AC30" s="43">
         <f t="shared" si="19"/>
-        <v>22.528480857142828</v>
-      </c>
-      <c r="AC30" s="28">
+        <v>19.275592114285697</v>
+      </c>
+      <c r="AD30" s="28">
         <f t="shared" si="20"/>
-        <v>19.275592114285697</v>
-      </c>
-      <c r="AD30" s="28">
+        <v>15.701847634285697</v>
+      </c>
+      <c r="AE30" s="28">
         <f t="shared" si="21"/>
-        <v>15.701847634285697</v>
-      </c>
-      <c r="AE30" s="28">
+        <v>20.053787340659387</v>
+      </c>
+      <c r="AF30" s="28">
         <f t="shared" si="22"/>
-        <v>20.053787340659387</v>
-      </c>
-      <c r="AF30" s="28">
+        <v>22.530655371428601</v>
+      </c>
+      <c r="AG30" s="28">
         <f t="shared" si="23"/>
-        <v>22.530655371428601</v>
-      </c>
-      <c r="AG30" s="28">
+        <v>25.002285749999999</v>
+      </c>
+      <c r="AH30" s="28">
         <f t="shared" si="24"/>
-        <v>25.002285749999999</v>
-      </c>
-      <c r="AH30" s="28">
+        <v>24.800940599999997</v>
+      </c>
+      <c r="AI30" s="28">
         <f t="shared" si="25"/>
-        <v>24.800940599999997</v>
-      </c>
-      <c r="AI30" s="28">
+        <v>25.305910000000036</v>
+      </c>
+      <c r="AJ30" s="28">
         <f t="shared" si="26"/>
-        <v>25.305910000000036</v>
-      </c>
-      <c r="AJ30" s="28">
+        <v>23.034445199999997</v>
+      </c>
+      <c r="AK30" s="43"/>
+      <c r="AL30" s="28">
         <f t="shared" si="27"/>
-        <v>23.034445199999997</v>
-      </c>
-      <c r="AK30" s="28"/>
-      <c r="AL30" s="28">
-        <f t="shared" si="28"/>
         <v>17.786401342468896</v>
       </c>
       <c r="AM30">
@@ -6483,20 +6598,16 @@
         <f t="shared" si="13"/>
         <v>8.0378250591016581E-2</v>
       </c>
-      <c r="AY30" t="e">
+      <c r="AZ30">
         <f t="shared" si="14"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AZ30">
-        <f t="shared" si="15"/>
         <v>1.2258834644749587E-2</v>
       </c>
       <c r="BA30">
-        <f t="shared" si="29"/>
+        <f t="shared" si="28"/>
         <v>6.9797836069996691E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:53" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:53" x14ac:dyDescent="0.4">
       <c r="A31" s="1">
         <v>2017</v>
       </c>
@@ -6570,59 +6681,59 @@
         <v>16.663797115277301</v>
       </c>
       <c r="Y31" s="28">
+        <f t="shared" si="15"/>
+        <v>23.160115714285698</v>
+      </c>
+      <c r="Z31" s="28">
         <f t="shared" si="16"/>
-        <v>23.160115714285698</v>
-      </c>
-      <c r="Z31" s="28">
+        <v>22.760764114285699</v>
+      </c>
+      <c r="AA31" s="43">
         <f t="shared" si="17"/>
-        <v>22.760764114285699</v>
-      </c>
-      <c r="AA31" s="28">
+        <v>19.346202285714266</v>
+      </c>
+      <c r="AB31" s="28">
         <f t="shared" si="18"/>
-        <v>19.346202285714266</v>
-      </c>
-      <c r="AB31" s="28">
+        <v>22.600178285714335</v>
+      </c>
+      <c r="AC31" s="43">
         <f t="shared" si="19"/>
-        <v>22.600178285714335</v>
-      </c>
-      <c r="AC31" s="28">
+        <v>19.667373942857097</v>
+      </c>
+      <c r="AD31" s="28">
         <f t="shared" si="20"/>
-        <v>19.667373942857097</v>
-      </c>
-      <c r="AD31" s="28">
+        <v>16.454812182857097</v>
+      </c>
+      <c r="AE31" s="28">
         <f t="shared" si="21"/>
-        <v>16.454812182857097</v>
-      </c>
-      <c r="AE31" s="28">
+        <v>20.373431472527507</v>
+      </c>
+      <c r="AF31" s="28">
         <f t="shared" si="22"/>
-        <v>20.373431472527507</v>
-      </c>
-      <c r="AF31" s="28">
+        <v>22.602291257142905</v>
+      </c>
+      <c r="AG31" s="28">
         <f t="shared" si="23"/>
-        <v>22.602291257142905</v>
-      </c>
-      <c r="AG31" s="28">
+        <v>24.826061624999998</v>
+      </c>
+      <c r="AH31" s="28">
         <f t="shared" si="24"/>
-        <v>24.826061624999998</v>
-      </c>
-      <c r="AH31" s="28">
+        <v>24.651345299999999</v>
+      </c>
+      <c r="AI31" s="28">
         <f t="shared" si="25"/>
-        <v>24.651345299999999</v>
-      </c>
-      <c r="AI31" s="28">
+        <v>25.331039999999998</v>
+      </c>
+      <c r="AJ31" s="28">
         <f t="shared" si="26"/>
-        <v>25.331039999999998</v>
-      </c>
-      <c r="AJ31" s="28">
+        <v>23.2199046</v>
+      </c>
+      <c r="AK31" s="43">
+        <f t="shared" ref="AK31:AK34" si="29">W31*1.077</f>
+        <v>19.2576216</v>
+      </c>
+      <c r="AL31" s="28">
         <f t="shared" si="27"/>
-        <v>23.2199046</v>
-      </c>
-      <c r="AK31" s="28">
-        <f t="shared" ref="AK31:AK34" si="30">W31*1.077</f>
-        <v>19.2576216</v>
-      </c>
-      <c r="AL31" s="28">
-        <f t="shared" si="28"/>
         <v>17.946909493153651</v>
       </c>
       <c r="AM31">
@@ -6673,20 +6784,16 @@
         <f t="shared" si="13"/>
         <v>8.0513942658362852E-3</v>
       </c>
-      <c r="AY31" t="e">
+      <c r="AZ31">
         <f t="shared" si="14"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AZ31">
-        <f t="shared" si="15"/>
         <v>9.0242060546282393E-3</v>
       </c>
       <c r="BA31">
-        <f t="shared" si="29"/>
+        <f t="shared" si="28"/>
         <v>9.3553539982954119E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:53" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:53" x14ac:dyDescent="0.4">
       <c r="A32" s="1">
         <v>2018</v>
       </c>
@@ -6759,59 +6866,59 @@
         <v>17.2112166978315</v>
       </c>
       <c r="Y32" s="28">
+        <f t="shared" si="15"/>
+        <v>23.463214285714297</v>
+      </c>
+      <c r="Z32" s="28">
         <f t="shared" si="16"/>
-        <v>23.463214285714297</v>
-      </c>
-      <c r="Z32" s="28">
+        <v>23.075494285714299</v>
+      </c>
+      <c r="AA32" s="43">
         <f t="shared" si="17"/>
-        <v>23.075494285714299</v>
-      </c>
-      <c r="AA32" s="28">
+        <v>19.760385714285771</v>
+      </c>
+      <c r="AB32" s="28">
         <f t="shared" si="18"/>
-        <v>19.760385714285771</v>
-      </c>
-      <c r="AB32" s="28">
+        <v>22.919585714285734</v>
+      </c>
+      <c r="AC32" s="43">
         <f t="shared" si="19"/>
-        <v>22.919585714285734</v>
-      </c>
-      <c r="AC32" s="28">
+        <v>20.072202857142905</v>
+      </c>
+      <c r="AD32" s="28">
         <f t="shared" si="20"/>
-        <v>20.072202857142905</v>
-      </c>
-      <c r="AD32" s="28">
+        <v>16.953210857142903</v>
+      </c>
+      <c r="AE32" s="28">
         <f t="shared" si="21"/>
-        <v>16.953210857142903</v>
-      </c>
-      <c r="AE32" s="28">
+        <v>20.757695604395632</v>
+      </c>
+      <c r="AF32" s="28">
         <f t="shared" si="22"/>
-        <v>20.757695604395632</v>
-      </c>
-      <c r="AF32" s="28">
+        <v>22.921637142857097</v>
+      </c>
+      <c r="AG32" s="28">
         <f t="shared" si="23"/>
-        <v>22.921637142857097</v>
-      </c>
-      <c r="AG32" s="28">
+        <v>25.080637500000002</v>
+      </c>
+      <c r="AH32" s="28">
         <f t="shared" si="24"/>
-        <v>25.080637500000002</v>
-      </c>
-      <c r="AH32" s="28">
+        <v>24.911009999999997</v>
+      </c>
+      <c r="AI32" s="28">
         <f t="shared" si="25"/>
-        <v>24.911009999999997</v>
-      </c>
-      <c r="AI32" s="28">
+        <v>25.381300000000032</v>
+      </c>
+      <c r="AJ32" s="28">
         <f t="shared" si="26"/>
-        <v>25.381300000000032</v>
-      </c>
-      <c r="AJ32" s="28">
+        <v>23.332343399999999</v>
+      </c>
+      <c r="AK32" s="43">
+        <f t="shared" si="29"/>
+        <v>19.818954000000002</v>
+      </c>
+      <c r="AL32" s="28">
         <f t="shared" si="27"/>
-        <v>23.332343399999999</v>
-      </c>
-      <c r="AK32" s="28">
-        <f t="shared" si="30"/>
-        <v>19.818954000000002</v>
-      </c>
-      <c r="AL32" s="28">
-        <f t="shared" si="28"/>
         <v>18.536480383564523</v>
       </c>
       <c r="AM32">
@@ -6863,26 +6970,35 @@
         <v>4.8423454763032048E-3</v>
       </c>
       <c r="AY32">
+        <f t="shared" ref="AY23:AY34" si="30">(W32-W31)/W31</f>
+        <v>2.9148583955975142E-2</v>
+      </c>
+      <c r="AZ32">
         <f t="shared" si="14"/>
-        <v>2.9148583955975142E-2</v>
-      </c>
-      <c r="AZ32">
-        <f t="shared" si="15"/>
         <v>3.285083098211309E-2</v>
       </c>
       <c r="BA32">
-        <f t="shared" si="29"/>
+        <f t="shared" si="28"/>
         <v>1.6852375794482774E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:53" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:54" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A33" s="1">
         <v>2019</v>
       </c>
-      <c r="B33" s="25"/>
-      <c r="E33" s="29">
-        <f>C32*(1-0.051)</f>
-        <v>2.3725000000000001</v>
+      <c r="B33" s="29">
+        <v>2498</v>
+      </c>
+      <c r="C33" s="29">
+        <v>2.1840000000000002</v>
+      </c>
+      <c r="D33" s="22">
+        <f t="shared" si="0"/>
+        <v>-0.12639999999999993</v>
+      </c>
+      <c r="E33" s="8">
+        <f>C33</f>
+        <v>2.1840000000000002</v>
       </c>
       <c r="F33" s="8"/>
       <c r="G33" s="8"/>
@@ -6932,59 +7048,59 @@
         <v>17.0428297528677</v>
       </c>
       <c r="Y33" s="28">
+        <f t="shared" si="15"/>
+        <v>23.277047142857093</v>
+      </c>
+      <c r="Z33" s="28">
         <f t="shared" si="16"/>
-        <v>23.277047142857093</v>
-      </c>
-      <c r="Z33" s="28">
+        <v>22.893204342857096</v>
+      </c>
+      <c r="AA33" s="43">
         <f t="shared" si="17"/>
-        <v>22.893204342857096</v>
-      </c>
-      <c r="AA33" s="28">
+        <v>19.611246857142902</v>
+      </c>
+      <c r="AB33" s="28">
         <f t="shared" si="18"/>
-        <v>19.611246857142902</v>
-      </c>
-      <c r="AB33" s="28">
+        <v>22.738854857142904</v>
+      </c>
+      <c r="AC33" s="43">
         <f t="shared" si="19"/>
-        <v>22.738854857142904</v>
-      </c>
-      <c r="AC33" s="28">
+        <v>19.919945828571397</v>
+      </c>
+      <c r="AD33" s="28">
         <f t="shared" si="20"/>
-        <v>19.919945828571397</v>
-      </c>
-      <c r="AD33" s="28">
+        <v>16.832143748571397</v>
+      </c>
+      <c r="AE33" s="28">
         <f t="shared" si="21"/>
-        <v>16.832143748571397</v>
-      </c>
-      <c r="AE33" s="28">
+        <v>20.598583648351639</v>
+      </c>
+      <c r="AF33" s="28">
         <f t="shared" si="22"/>
-        <v>20.598583648351639</v>
-      </c>
-      <c r="AF33" s="28">
+        <v>22.740885771428601</v>
+      </c>
+      <c r="AG33" s="28">
         <f t="shared" si="23"/>
-        <v>22.740885771428601</v>
-      </c>
-      <c r="AG33" s="28">
+        <v>24.878296124999999</v>
+      </c>
+      <c r="AH33" s="28">
         <f t="shared" si="24"/>
-        <v>24.878296124999999</v>
-      </c>
-      <c r="AH33" s="28">
+        <v>24.710364899999998</v>
+      </c>
+      <c r="AI33" s="28">
         <f t="shared" si="25"/>
-        <v>24.710364899999998</v>
-      </c>
-      <c r="AI33" s="28">
+        <v>24.975629999999999</v>
+      </c>
+      <c r="AJ33" s="28">
         <f t="shared" si="26"/>
-        <v>24.975629999999999</v>
-      </c>
-      <c r="AJ33" s="28">
+        <v>23.145053100000002</v>
+      </c>
+      <c r="AK33" s="43">
+        <f t="shared" si="29"/>
+        <v>19.618775599999964</v>
+      </c>
+      <c r="AL33" s="28">
         <f t="shared" si="27"/>
-        <v>23.145053100000002</v>
-      </c>
-      <c r="AK33" s="28">
-        <f t="shared" si="30"/>
-        <v>19.618775599999964</v>
-      </c>
-      <c r="AL33" s="28">
-        <f t="shared" si="28"/>
         <v>18.355127643838511</v>
       </c>
       <c r="AM33">
@@ -7036,328 +7152,614 @@
         <v>-8.0270676969377928E-3</v>
       </c>
       <c r="AY33">
+        <f t="shared" si="30"/>
+        <v>-1.0100351411080385E-2</v>
+      </c>
+      <c r="AZ33">
         <f t="shared" si="14"/>
-        <v>-1.0100351411080385E-2</v>
-      </c>
-      <c r="AZ33">
+        <v>-9.7835584735282092E-3</v>
+      </c>
+      <c r="BA33">
+        <f t="shared" si="28"/>
+        <v>-8.6828999057985794E-3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:54" s="33" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A34" s="32">
+        <v>2020</v>
+      </c>
+      <c r="E34" s="34">
+        <f>E33*(1+$D$3)</f>
+        <v>2.0516034507602341</v>
+      </c>
+      <c r="K34" s="35">
+        <v>21.2128571428571</v>
+      </c>
+      <c r="L34" s="35">
+        <v>20.856457142857099</v>
+      </c>
+      <c r="M34" s="35">
+        <v>17.809142857142898</v>
+      </c>
+      <c r="N34" s="35">
+        <v>20.713142857142898</v>
+      </c>
+      <c r="O34" s="35">
+        <v>18.0957714285714</v>
+      </c>
+      <c r="P34" s="35">
+        <v>15.2287314285714</v>
+      </c>
+      <c r="Q34" s="35">
+        <v>18.725890109890099</v>
+      </c>
+      <c r="R34" s="35">
+        <v>20.715028571428601</v>
+      </c>
+      <c r="S34" s="35">
+        <v>22.699625000000001</v>
+      </c>
+      <c r="T34" s="35">
+        <v>22.543700000000001</v>
+      </c>
+      <c r="U34" s="35">
+        <v>22.601666666666699</v>
+      </c>
+      <c r="V34" s="35">
+        <v>21.090299999999999</v>
+      </c>
+      <c r="W34" s="35">
+        <v>17.816133333333301</v>
+      </c>
+      <c r="X34" s="35">
+        <v>16.642829752867701</v>
+      </c>
+      <c r="Y34" s="36">
         <f t="shared" si="15"/>
-        <v>-9.7835584735282092E-3</v>
-      </c>
-      <c r="BA33">
+        <v>22.846247142857095</v>
+      </c>
+      <c r="Z34" s="36">
+        <f t="shared" si="16"/>
+        <v>22.462404342857095</v>
+      </c>
+      <c r="AA34" s="44">
+        <f t="shared" si="17"/>
+        <v>19.180446857142901</v>
+      </c>
+      <c r="AB34" s="36">
+        <f t="shared" si="18"/>
+        <v>22.308054857142899</v>
+      </c>
+      <c r="AC34" s="44">
+        <f t="shared" si="19"/>
+        <v>19.489145828571395</v>
+      </c>
+      <c r="AD34" s="36">
+        <f t="shared" si="20"/>
+        <v>16.401343748571399</v>
+      </c>
+      <c r="AE34" s="36">
+        <f t="shared" si="21"/>
+        <v>20.167783648351634</v>
+      </c>
+      <c r="AF34" s="36">
+        <f t="shared" si="22"/>
+        <v>22.310085771428604</v>
+      </c>
+      <c r="AG34" s="36">
+        <f t="shared" si="23"/>
+        <v>24.447496125000001</v>
+      </c>
+      <c r="AH34" s="36">
+        <f t="shared" si="24"/>
+        <v>24.2795649</v>
+      </c>
+      <c r="AI34" s="36">
+        <f t="shared" si="25"/>
+        <v>24.341995000000033</v>
+      </c>
+      <c r="AJ34" s="36">
+        <f t="shared" si="26"/>
+        <v>22.714253099999997</v>
+      </c>
+      <c r="AK34" s="44">
         <f t="shared" si="29"/>
-        <v>-8.6828999057985794E-3</v>
-      </c>
-    </row>
-    <row r="34" spans="1:53" x14ac:dyDescent="0.35">
-      <c r="A34" s="1">
-        <v>2020</v>
-      </c>
-      <c r="B34" s="25"/>
-      <c r="E34" s="29">
-        <f t="shared" ref="E34:E49" si="31">E33*(1-0.051)</f>
-        <v>2.2515025</v>
-      </c>
-      <c r="K34" s="7">
-        <v>21.2128571428571</v>
-      </c>
-      <c r="L34" s="7">
-        <v>20.856457142857099</v>
-      </c>
-      <c r="M34" s="7">
-        <v>17.809142857142898</v>
-      </c>
-      <c r="N34" s="7">
-        <v>20.713142857142898</v>
-      </c>
-      <c r="O34" s="7">
-        <v>18.0957714285714</v>
-      </c>
-      <c r="P34" s="7">
-        <v>15.2287314285714</v>
-      </c>
-      <c r="Q34" s="7">
-        <v>18.725890109890099</v>
-      </c>
-      <c r="R34" s="7">
-        <v>20.715028571428601</v>
-      </c>
-      <c r="S34" s="7">
-        <v>22.699625000000001</v>
-      </c>
-      <c r="T34" s="7">
-        <v>22.543700000000001</v>
-      </c>
-      <c r="U34" s="7">
-        <v>22.601666666666699</v>
-      </c>
-      <c r="V34" s="7">
-        <v>21.090299999999999</v>
-      </c>
-      <c r="W34" s="7">
-        <v>17.816133333333301</v>
-      </c>
-      <c r="X34" s="7">
-        <v>16.642829752867701</v>
-      </c>
-      <c r="Y34" s="28">
-        <f t="shared" si="16"/>
-        <v>22.846247142857095</v>
-      </c>
-      <c r="Z34" s="28">
-        <f t="shared" si="17"/>
-        <v>22.462404342857095</v>
-      </c>
-      <c r="AA34" s="28">
-        <f t="shared" si="18"/>
-        <v>19.180446857142901</v>
-      </c>
-      <c r="AB34" s="28">
-        <f t="shared" si="19"/>
-        <v>22.308054857142899</v>
-      </c>
-      <c r="AC34" s="28">
-        <f t="shared" si="20"/>
-        <v>19.489145828571395</v>
-      </c>
-      <c r="AD34" s="28">
-        <f t="shared" si="21"/>
-        <v>16.401343748571399</v>
-      </c>
-      <c r="AE34" s="28">
-        <f t="shared" si="22"/>
-        <v>20.167783648351634</v>
-      </c>
-      <c r="AF34" s="28">
-        <f t="shared" si="23"/>
-        <v>22.310085771428604</v>
-      </c>
-      <c r="AG34" s="28">
-        <f t="shared" si="24"/>
-        <v>24.447496125000001</v>
-      </c>
-      <c r="AH34" s="28">
-        <f t="shared" si="25"/>
-        <v>24.2795649</v>
-      </c>
-      <c r="AI34" s="28">
-        <f t="shared" si="26"/>
-        <v>24.341995000000033</v>
-      </c>
-      <c r="AJ34" s="28">
+        <v>19.187975599999966</v>
+      </c>
+      <c r="AL34" s="36">
         <f t="shared" si="27"/>
-        <v>22.714253099999997</v>
-      </c>
-      <c r="AK34" s="28">
-        <f t="shared" si="30"/>
-        <v>19.187975599999966</v>
-      </c>
-      <c r="AL34" s="28">
-        <f t="shared" si="28"/>
         <v>17.924327643838513</v>
       </c>
-      <c r="AM34">
+      <c r="AM34" s="33">
         <f t="shared" si="2"/>
         <v>-1.8507502148192186E-2</v>
       </c>
-      <c r="AN34">
+      <c r="AN34" s="33">
         <f t="shared" si="3"/>
         <v>-1.8817811327247254E-2</v>
       </c>
-      <c r="AO34">
+      <c r="AO34" s="33">
         <f t="shared" si="4"/>
         <v>-2.1966986757045191E-2</v>
       </c>
-      <c r="AP34">
+      <c r="AP34" s="33">
         <f t="shared" si="5"/>
         <v>-1.8945545090397378E-2</v>
       </c>
-      <c r="AQ34">
+      <c r="AQ34" s="33">
         <f t="shared" si="6"/>
         <v>-2.1626564836441337E-2</v>
       </c>
-      <c r="AR34">
+      <c r="AR34" s="33">
         <f t="shared" si="7"/>
         <v>-2.5593887887071062E-2</v>
       </c>
-      <c r="AS34">
+      <c r="AS34" s="33">
         <f t="shared" si="8"/>
         <v>-2.0914059303998613E-2</v>
       </c>
-      <c r="AT34">
+      <c r="AT34" s="33">
         <f t="shared" si="9"/>
         <v>-1.894385312560036E-2</v>
       </c>
-      <c r="AU34">
+      <c r="AU34" s="33">
         <f t="shared" si="10"/>
         <v>-1.7316298424757917E-2</v>
       </c>
-      <c r="AV34">
+      <c r="AV34" s="33">
         <f t="shared" si="11"/>
         <v>-1.743397969813058E-2</v>
       </c>
-      <c r="AW34">
+      <c r="AW34" s="33">
         <f t="shared" si="12"/>
         <v>-2.5370130803505937E-2</v>
       </c>
-      <c r="AX34">
+      <c r="AX34" s="33">
         <f t="shared" si="13"/>
         <v>-1.8613048677775652E-2</v>
       </c>
-      <c r="AY34">
+      <c r="AY34" s="33">
+        <f t="shared" si="30"/>
+        <v>-2.195855688364157E-2</v>
+      </c>
+      <c r="AZ34" s="33">
         <f t="shared" si="14"/>
-        <v>-2.195855688364157E-2</v>
-      </c>
-      <c r="AZ34">
-        <f t="shared" si="15"/>
         <v>-2.3470280804318476E-2</v>
       </c>
-      <c r="BA34">
-        <f t="shared" si="29"/>
+      <c r="BA34" s="33">
+        <f t="shared" si="28"/>
         <v>-2.0677036126294537E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:53" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:54" x14ac:dyDescent="0.4">
       <c r="A35" s="1">
         <v>2021</v>
       </c>
       <c r="E35" s="29">
-        <f t="shared" si="31"/>
-        <v>2.1366758724999997</v>
-      </c>
-    </row>
-    <row r="36" spans="1:53" x14ac:dyDescent="0.35">
+        <f t="shared" ref="E35:E49" si="31">E34*(1+$D$3)</f>
+        <v>1.9272329300234889</v>
+      </c>
+    </row>
+    <row r="36" spans="1:54" x14ac:dyDescent="0.4">
       <c r="A36" s="1">
         <v>2022</v>
       </c>
       <c r="E36" s="29">
         <f t="shared" si="31"/>
-        <v>2.0277054030024995</v>
-      </c>
-    </row>
-    <row r="37" spans="1:53" x14ac:dyDescent="0.35">
+        <v>1.8104018908676494</v>
+      </c>
+    </row>
+    <row r="37" spans="1:54" x14ac:dyDescent="0.4">
       <c r="A37" s="1">
         <v>2023</v>
       </c>
       <c r="E37" s="29">
         <f t="shared" si="31"/>
-        <v>1.9242924274493718</v>
-      </c>
-    </row>
-    <row r="38" spans="1:53" x14ac:dyDescent="0.35">
+        <v>1.7006532813951107</v>
+      </c>
+      <c r="BA37" t="s">
+        <v>122</v>
+      </c>
+      <c r="BB37" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="38" spans="1:54" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A38" s="1">
         <v>2024</v>
       </c>
       <c r="E38" s="29">
         <f t="shared" si="31"/>
-        <v>1.8261535136494538</v>
-      </c>
-    </row>
-    <row r="39" spans="1:53" x14ac:dyDescent="0.35">
+        <v>1.5975577567110459</v>
+      </c>
+      <c r="AL38" t="s">
+        <v>118</v>
+      </c>
+      <c r="AM38" s="38">
+        <f>AVERAGE(AM29:AM33)</f>
+        <v>5.7524590877006808E-2</v>
+      </c>
+      <c r="AN38" s="38">
+        <f t="shared" ref="AN38:AZ38" si="32">AVERAGE(AN29:AN33)</f>
+        <v>5.8322354677273057E-2</v>
+      </c>
+      <c r="AO38" s="22">
+        <f t="shared" si="32"/>
+        <v>6.6171486326797077E-2</v>
+      </c>
+      <c r="AP38" s="38">
+        <f t="shared" si="32"/>
+        <v>5.8625219637744905E-2</v>
+      </c>
+      <c r="AQ38" s="22">
+        <f t="shared" si="32"/>
+        <v>6.5337544922938251E-2</v>
+      </c>
+      <c r="AR38" s="38">
+        <f t="shared" si="32"/>
+        <v>7.5870078215146353E-2</v>
+      </c>
+      <c r="AS38" s="38">
+        <f t="shared" si="32"/>
+        <v>6.5327982157697223E-2</v>
+      </c>
+      <c r="AT38" s="38">
+        <f t="shared" si="32"/>
+        <v>5.8622909134773672E-2</v>
+      </c>
+      <c r="AU38" s="38">
+        <f t="shared" si="32"/>
+        <v>5.4579311197457035E-2</v>
+      </c>
+      <c r="AV38" s="38">
+        <f t="shared" si="32"/>
+        <v>5.4820273756141923E-2</v>
+      </c>
+      <c r="AW38" s="38">
+        <f t="shared" si="32"/>
+        <v>4.3901226002016888E-2</v>
+      </c>
+      <c r="AX38" s="38">
+        <f t="shared" si="32"/>
+        <v>5.2976844212830478E-2</v>
+      </c>
+      <c r="AY38" s="22">
+        <f t="shared" si="32"/>
+        <v>9.524116272447378E-3</v>
+      </c>
+      <c r="AZ38" s="38">
+        <f t="shared" si="32"/>
+        <v>4.2500708704996656E-2</v>
+      </c>
+      <c r="BA38" s="37">
+        <f>AVERAGE(AM38:AZ38)</f>
+        <v>5.4578903292519125E-2</v>
+      </c>
+      <c r="BB38" s="37">
+        <f>AVERAGE(AM38,AN38,AP38,AR38,AS38,AT38, AU38,AV38,AW38,AX38,AZ38)</f>
+        <v>5.6642863506644089E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:54" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A39" s="1">
         <v>2025</v>
       </c>
       <c r="E39" s="29">
         <f t="shared" si="31"/>
-        <v>1.7330196844533317</v>
-      </c>
-    </row>
-    <row r="40" spans="1:53" x14ac:dyDescent="0.35">
+        <v>1.5007119992935714</v>
+      </c>
+      <c r="AL39" t="s">
+        <v>119</v>
+      </c>
+      <c r="AM39" s="38">
+        <f>AVERAGE(AM32:AM33)</f>
+        <v>2.5763330222278837E-3</v>
+      </c>
+      <c r="AN39" s="38">
+        <f t="shared" ref="AN39:AZ39" si="33">AVERAGE(AN32:AN33)</f>
+        <v>2.9640153580081105E-3</v>
+      </c>
+      <c r="AO39" s="22">
+        <f t="shared" si="33"/>
+        <v>6.9308322446428195E-3</v>
+      </c>
+      <c r="AP39" s="38">
+        <f t="shared" si="33"/>
+        <v>3.1237637932709714E-3</v>
+      </c>
+      <c r="AQ39" s="22">
+        <f t="shared" si="33"/>
+        <v>6.4991569985399043E-3</v>
+      </c>
+      <c r="AR39" s="38">
+        <f t="shared" si="33"/>
+        <v>1.1573840854746817E-2</v>
+      </c>
+      <c r="AS39" s="38">
+        <f t="shared" si="33"/>
+        <v>5.5979190056546215E-3</v>
+      </c>
+      <c r="AT39" s="38">
+        <f t="shared" si="33"/>
+        <v>3.1216471307288739E-3</v>
+      </c>
+      <c r="AU39" s="38">
+        <f t="shared" si="33"/>
+        <v>1.093373679483681E-3</v>
+      </c>
+      <c r="AV39" s="38">
+        <f t="shared" si="33"/>
+        <v>1.239507662057597E-3</v>
+      </c>
+      <c r="AW39" s="38">
+        <f t="shared" si="33"/>
+        <v>-6.9994499449944521E-3</v>
+      </c>
+      <c r="AX39" s="38">
+        <f t="shared" si="33"/>
+        <v>-1.592361110317294E-3</v>
+      </c>
+      <c r="AY39" s="22">
+        <f t="shared" si="33"/>
+        <v>9.524116272447378E-3</v>
+      </c>
+      <c r="AZ39" s="38">
+        <f t="shared" si="33"/>
+        <v>1.1533636254292441E-2</v>
+      </c>
+      <c r="BA39" s="45">
+        <f>AVERAGE(AM39:AZ39)</f>
+        <v>4.0847379443420965E-3</v>
+      </c>
+      <c r="BB39" s="46">
+        <f t="shared" ref="BB39:BB41" si="34">AVERAGE(AM39,AN39,AP39,AR39,AS39,AT39, AU39,AV39,AW39,AX39,AZ39)</f>
+        <v>3.1120205186508415E-3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:54" x14ac:dyDescent="0.4">
       <c r="A40" s="1">
         <v>2026</v>
       </c>
       <c r="E40" s="29">
         <f t="shared" si="31"/>
-        <v>1.6446356805462117</v>
-      </c>
-    </row>
-    <row r="41" spans="1:53" x14ac:dyDescent="0.35">
+        <v>1.4097371411849728</v>
+      </c>
+      <c r="AL40" t="s">
+        <v>120</v>
+      </c>
+      <c r="AM40" s="38">
+        <f>AVERAGE(AM30:AM34)</f>
+        <v>1.1477207120931338E-2</v>
+      </c>
+      <c r="AN40" s="38">
+        <f t="shared" ref="AN40:BA40" si="35">AVERAGE(AN30:AN34)</f>
+        <v>1.1978953630635185E-2</v>
+      </c>
+      <c r="AO40" s="22">
+        <f t="shared" si="35"/>
+        <v>1.7256819862172118E-2</v>
+      </c>
+      <c r="AP40" s="38">
+        <f t="shared" si="35"/>
+        <v>1.2164921725611805E-2</v>
+      </c>
+      <c r="AQ40" s="22">
+        <f t="shared" si="35"/>
+        <v>1.667028498848085E-2</v>
+      </c>
+      <c r="AR40" s="38">
+        <f t="shared" si="35"/>
+        <v>2.3656181943781114E-2</v>
+      </c>
+      <c r="AS40" s="38">
+        <f t="shared" si="35"/>
+        <v>2.3039372405649888E-2</v>
+      </c>
+      <c r="AT40" s="38">
+        <f t="shared" si="35"/>
+        <v>1.216381279995625E-2</v>
+      </c>
+      <c r="AU40" s="38">
+        <f t="shared" si="35"/>
+        <v>9.528952709189395E-3</v>
+      </c>
+      <c r="AV40" s="38">
+        <f t="shared" si="35"/>
+        <v>9.7788607303622623E-3</v>
+      </c>
+      <c r="AW40" s="38">
+        <f t="shared" si="35"/>
+        <v>6.1414411908122697E-3</v>
+      </c>
+      <c r="AX40" s="38">
+        <f t="shared" si="35"/>
+        <v>1.3326374791688526E-2</v>
+      </c>
+      <c r="AY40" s="22">
+        <f t="shared" si="35"/>
+        <v>-9.7010811291560473E-4</v>
+      </c>
+      <c r="AZ40" s="38">
+        <f t="shared" si="35"/>
+        <v>4.1760064807288468E-3</v>
+      </c>
+      <c r="BA40" s="37">
+        <f t="shared" ref="BA40:BA41" si="36">AVERAGE(AM40:AZ40)</f>
+        <v>1.2170648733363163E-2</v>
+      </c>
+      <c r="BB40" s="37">
+        <f t="shared" si="34"/>
+        <v>1.2493825957213352E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:54" x14ac:dyDescent="0.4">
       <c r="A41" s="1">
         <v>2027</v>
       </c>
       <c r="E41" s="29">
         <f t="shared" si="31"/>
-        <v>1.5607592608383547</v>
-      </c>
-    </row>
-    <row r="42" spans="1:53" x14ac:dyDescent="0.35">
+        <v>1.3242772818314823</v>
+      </c>
+      <c r="AL41" t="s">
+        <v>121</v>
+      </c>
+      <c r="AM41" s="38">
+        <f>AVERAGE(AM33:AM34)</f>
+        <v>-1.3220964188851509E-2</v>
+      </c>
+      <c r="AN41" s="38">
+        <f t="shared" ref="AN41:BA41" si="37">AVERAGE(AN33:AN34)</f>
+        <v>-1.3358765644955757E-2</v>
+      </c>
+      <c r="AO41" s="22">
+        <f t="shared" si="37"/>
+        <v>-1.4757176223059592E-2</v>
+      </c>
+      <c r="AP41" s="38">
+        <f t="shared" si="37"/>
+        <v>-1.3415489036583201E-2</v>
+      </c>
+      <c r="AQ41" s="22">
+        <f t="shared" si="37"/>
+        <v>-1.4606015823097717E-2</v>
+      </c>
+      <c r="AR41" s="38">
+        <f t="shared" si="37"/>
+        <v>-1.6367568693964329E-2</v>
+      </c>
+      <c r="AS41" s="38">
+        <f t="shared" si="37"/>
+        <v>-1.4289631282651899E-2</v>
+      </c>
+      <c r="AT41" s="38">
+        <f t="shared" si="37"/>
+        <v>-1.3414737678384518E-2</v>
+      </c>
+      <c r="AU41" s="38">
+        <f t="shared" si="37"/>
+        <v>-1.2691965637499769E-2</v>
+      </c>
+      <c r="AV41" s="38">
+        <f t="shared" si="37"/>
+        <v>-1.2744227203150877E-2</v>
+      </c>
+      <c r="AW41" s="38">
+        <f t="shared" si="37"/>
+        <v>-2.0676578838811598E-2</v>
+      </c>
+      <c r="AX41" s="38">
+        <f t="shared" si="37"/>
+        <v>-1.3320058187356723E-2</v>
+      </c>
+      <c r="AY41" s="22">
+        <f t="shared" si="37"/>
+        <v>-1.6029454147360976E-2</v>
+      </c>
+      <c r="AZ41" s="38">
+        <f t="shared" si="37"/>
+        <v>-1.6626919638923342E-2</v>
+      </c>
+      <c r="BA41" s="37">
+        <f t="shared" si="36"/>
+        <v>-1.467996801604656E-2</v>
+      </c>
+      <c r="BB41" s="37">
+        <f t="shared" si="34"/>
+        <v>-1.4556991457375774E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:54" x14ac:dyDescent="0.4">
       <c r="A42" s="1">
         <v>2028</v>
       </c>
       <c r="E42" s="29">
         <f t="shared" si="31"/>
-        <v>1.4811605385355986</v>
-      </c>
-    </row>
-    <row r="43" spans="1:53" x14ac:dyDescent="0.35">
+        <v>1.2439980957732839</v>
+      </c>
+    </row>
+    <row r="43" spans="1:54" x14ac:dyDescent="0.4">
       <c r="A43" s="1">
         <v>2029</v>
       </c>
       <c r="E43" s="29">
         <f t="shared" si="31"/>
-        <v>1.4056213510702831</v>
-      </c>
-    </row>
-    <row r="44" spans="1:53" x14ac:dyDescent="0.35">
+        <v>1.1685855247379255</v>
+      </c>
+    </row>
+    <row r="44" spans="1:54" x14ac:dyDescent="0.4">
       <c r="A44" s="1">
         <v>2030</v>
       </c>
       <c r="E44" s="29">
         <f t="shared" si="31"/>
-        <v>1.3339346621656987</v>
-      </c>
-    </row>
-    <row r="45" spans="1:53" x14ac:dyDescent="0.35">
+        <v>1.0977445490205067</v>
+      </c>
+    </row>
+    <row r="45" spans="1:54" x14ac:dyDescent="0.4">
       <c r="A45" s="1">
         <v>2031</v>
       </c>
       <c r="E45" s="29">
         <f t="shared" si="31"/>
-        <v>1.2659039943952479</v>
-      </c>
-    </row>
-    <row r="46" spans="1:53" x14ac:dyDescent="0.35">
+        <v>1.0311980333441888</v>
+      </c>
+    </row>
+    <row r="46" spans="1:54" x14ac:dyDescent="0.4">
       <c r="A46" s="1">
         <v>2032</v>
       </c>
       <c r="E46" s="29">
         <f t="shared" si="31"/>
-        <v>1.2013428906810901</v>
-      </c>
-    </row>
-    <row r="47" spans="1:53" x14ac:dyDescent="0.35">
+        <v>0.96868564268594526</v>
+      </c>
+    </row>
+    <row r="47" spans="1:54" x14ac:dyDescent="0.4">
       <c r="A47" s="1">
         <v>2033</v>
       </c>
       <c r="E47" s="29">
         <f t="shared" si="31"/>
-        <v>1.1400744032563546</v>
-      </c>
-    </row>
-    <row r="48" spans="1:53" x14ac:dyDescent="0.35">
+        <v>0.90996282382618143</v>
+      </c>
+    </row>
+    <row r="48" spans="1:54" x14ac:dyDescent="0.4">
       <c r="A48" s="1">
         <v>2034</v>
       </c>
       <c r="E48" s="29">
         <f t="shared" si="31"/>
-        <v>1.0819306086902805</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+        <v>0.85479984863796732</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A49" s="1">
         <v>2035</v>
       </c>
       <c r="E49" s="29">
         <f t="shared" si="31"/>
-        <v>1.026752147647076</v>
+        <v>0.80298091537315908</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="AM26:BA34">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="max"/>
+        <color rgb="FF5A8AC6"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="Z1" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
   <drawing r:id="rId3"/>
+  <legacyDrawing r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -7366,12 +7768,12 @@
   <dimension ref="B2:AC29"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P45" sqref="P45"/>
+      <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="2" spans="2:26" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:26" x14ac:dyDescent="0.4">
       <c r="B2" s="19" t="s">
         <v>49</v>
       </c>
@@ -7394,7 +7796,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="2:26" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:26" x14ac:dyDescent="0.4">
       <c r="U3">
         <v>0</v>
       </c>
@@ -7415,7 +7817,7 @@
         <v>-0.26400000000000001</v>
       </c>
     </row>
-    <row r="4" spans="2:26" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:26" x14ac:dyDescent="0.4">
       <c r="U4">
         <v>1</v>
       </c>
@@ -7439,7 +7841,7 @@
         <v>-0.26400000000000001</v>
       </c>
     </row>
-    <row r="5" spans="2:26" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:26" x14ac:dyDescent="0.4">
       <c r="U5">
         <v>2</v>
       </c>
@@ -7452,7 +7854,7 @@
         <v>1.5294246346336056</v>
       </c>
     </row>
-    <row r="6" spans="2:26" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:26" x14ac:dyDescent="0.4">
       <c r="U6">
         <v>3</v>
       </c>
@@ -7465,7 +7867,7 @@
         <v>1.3741684991995822</v>
       </c>
     </row>
-    <row r="7" spans="2:26" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:26" x14ac:dyDescent="0.4">
       <c r="U7">
         <v>4</v>
       </c>
@@ -7478,7 +7880,7 @@
         <v>1.2736677791107027</v>
       </c>
     </row>
-    <row r="8" spans="2:26" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:26" x14ac:dyDescent="0.4">
       <c r="U8">
         <v>5</v>
       </c>
@@ -7491,7 +7893,7 @@
         <v>1.2008034274852089</v>
       </c>
     </row>
-    <row r="9" spans="2:26" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:26" x14ac:dyDescent="0.4">
       <c r="U9">
         <v>6</v>
       </c>
@@ -7504,7 +7906,7 @@
         <v>1.144374231240699</v>
       </c>
     </row>
-    <row r="10" spans="2:26" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:26" x14ac:dyDescent="0.4">
       <c r="U10">
         <v>7</v>
       </c>
@@ -7517,7 +7919,7 @@
         <v>1.0987379304981457</v>
       </c>
     </row>
-    <row r="11" spans="2:26" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:26" x14ac:dyDescent="0.4">
       <c r="U11">
         <v>8</v>
       </c>
@@ -7530,7 +7932,7 @@
         <v>1.0606796665946323</v>
       </c>
     </row>
-    <row r="12" spans="2:26" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:26" x14ac:dyDescent="0.4">
       <c r="U12">
         <v>9</v>
       </c>
@@ -7543,7 +7945,7 @@
         <v>1.0282056299187541</v>
       </c>
     </row>
-    <row r="13" spans="2:26" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:26" x14ac:dyDescent="0.4">
       <c r="U13">
         <v>10</v>
       </c>
@@ -7556,7 +7958,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:26" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:26" x14ac:dyDescent="0.4">
       <c r="U14">
         <v>20</v>
       </c>
@@ -7569,7 +7971,7 @@
         <v>0.83277577088054899</v>
       </c>
     </row>
-    <row r="15" spans="2:26" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:26" x14ac:dyDescent="0.4">
       <c r="U15">
         <v>30</v>
       </c>
@@ -7582,7 +7984,7 @@
         <v>0.74823839326666097</v>
       </c>
     </row>
-    <row r="16" spans="2:26" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:26" x14ac:dyDescent="0.4">
       <c r="U16">
         <v>40</v>
       </c>
@@ -7595,7 +7997,7 @@
         <v>0.69351548456569256</v>
       </c>
     </row>
-    <row r="17" spans="21:29" x14ac:dyDescent="0.35">
+    <row r="17" spans="21:29" x14ac:dyDescent="0.4">
       <c r="U17">
         <v>50</v>
       </c>
@@ -7608,7 +8010,7 @@
         <v>0.65384065180796802</v>
       </c>
     </row>
-    <row r="18" spans="21:29" x14ac:dyDescent="0.35">
+    <row r="18" spans="21:29" x14ac:dyDescent="0.4">
       <c r="U18">
         <v>100</v>
       </c>
@@ -7621,7 +8023,7 @@
         <v>0.54450265284242116</v>
       </c>
     </row>
-    <row r="19" spans="21:29" x14ac:dyDescent="0.35">
+    <row r="19" spans="21:29" x14ac:dyDescent="0.4">
       <c r="U19">
         <v>200</v>
       </c>
@@ -7634,7 +8036,7 @@
         <v>0.4534486164673513</v>
       </c>
     </row>
-    <row r="20" spans="21:29" x14ac:dyDescent="0.35">
+    <row r="20" spans="21:29" x14ac:dyDescent="0.4">
       <c r="U20">
         <v>300</v>
       </c>
@@ -7647,7 +8049,7 @@
         <v>0.40741779009224771</v>
       </c>
     </row>
-    <row r="21" spans="21:29" x14ac:dyDescent="0.35">
+    <row r="21" spans="21:29" x14ac:dyDescent="0.4">
       <c r="U21">
         <v>500</v>
       </c>
@@ -7660,10 +8062,10 @@
         <v>0.35601796944565639</v>
       </c>
     </row>
-    <row r="22" spans="21:29" x14ac:dyDescent="0.35">
+    <row r="22" spans="21:29" x14ac:dyDescent="0.4">
       <c r="V22" s="7"/>
     </row>
-    <row r="23" spans="21:29" x14ac:dyDescent="0.35">
+    <row r="23" spans="21:29" x14ac:dyDescent="0.4">
       <c r="AA23" t="s">
         <v>69</v>
       </c>
@@ -7676,7 +8078,7 @@
         <v>1.986667714406829</v>
       </c>
     </row>
-    <row r="24" spans="21:29" x14ac:dyDescent="0.35">
+    <row r="24" spans="21:29" x14ac:dyDescent="0.4">
       <c r="U24" t="s">
         <v>58</v>
       </c>
@@ -7705,7 +8107,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="25" spans="21:29" x14ac:dyDescent="0.35">
+    <row r="25" spans="21:29" x14ac:dyDescent="0.4">
       <c r="U25">
         <v>2</v>
       </c>
@@ -7736,7 +8138,7 @@
         <v>1.929563156112428</v>
       </c>
     </row>
-    <row r="26" spans="21:29" x14ac:dyDescent="0.35">
+    <row r="26" spans="21:29" x14ac:dyDescent="0.4">
       <c r="U26">
         <v>10</v>
       </c>
@@ -7767,7 +8169,7 @@
         <v>2.1156278229448962</v>
       </c>
     </row>
-    <row r="27" spans="21:29" x14ac:dyDescent="0.35">
+    <row r="27" spans="21:29" x14ac:dyDescent="0.4">
       <c r="U27">
         <v>30</v>
       </c>
@@ -7798,7 +8200,7 @@
         <v>2.2026431718061672</v>
       </c>
     </row>
-    <row r="28" spans="21:29" x14ac:dyDescent="0.35">
+    <row r="28" spans="21:29" x14ac:dyDescent="0.4">
       <c r="U28">
         <v>100</v>
       </c>
@@ -7829,7 +8231,7 @@
         <v>2.3114886731391584</v>
       </c>
     </row>
-    <row r="29" spans="21:29" x14ac:dyDescent="0.35">
+    <row r="29" spans="21:29" x14ac:dyDescent="0.4">
       <c r="U29" s="20" t="s">
         <v>59</v>
       </c>
@@ -7873,20 +8275,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.90625" customWidth="1"/>
-    <col min="4" max="4" width="43.54296875" customWidth="1"/>
-    <col min="5" max="5" width="41.54296875" customWidth="1"/>
+    <col min="1" max="1" width="10.15234375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.15234375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.921875" customWidth="1"/>
+    <col min="4" max="4" width="43.53515625" customWidth="1"/>
+    <col min="5" max="5" width="41.53515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
@@ -7899,7 +8301,7 @@
       <c r="D1" s="6"/>
       <c r="E1" s="6"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>43</v>
       </c>
@@ -7912,7 +8314,7 @@
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
         <v>48</v>
       </c>
@@ -7923,7 +8325,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
         <v>51</v>
       </c>
@@ -7935,7 +8337,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A5" s="2" t="s">
         <v>82</v>
       </c>
@@ -7946,21 +8348,21 @@
         <v>84</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A10" s="11"/>
       <c r="B10" s="12" t="s">
         <v>10</v>
       </c>
       <c r="C10" s="13"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A11" s="11"/>
       <c r="B11" s="13" t="s">
         <v>11</v>
       </c>
       <c r="C11" s="13"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A12" s="15" t="s">
         <v>12</v>
       </c>
@@ -7969,7 +8371,7 @@
       </c>
       <c r="C12" s="16"/>
     </row>
-    <row r="13" spans="1:5" ht="23" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" ht="23.15" x14ac:dyDescent="0.4">
       <c r="A13" s="15" t="s">
         <v>15</v>
       </c>
@@ -7980,7 +8382,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="23" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" ht="23.15" x14ac:dyDescent="0.4">
       <c r="A14" s="15" t="s">
         <v>18</v>
       </c>
@@ -7991,7 +8393,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" ht="34.75" x14ac:dyDescent="0.4">
       <c r="A15" s="15" t="s">
         <v>21</v>
       </c>
@@ -8002,7 +8404,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" ht="34.75" x14ac:dyDescent="0.4">
       <c r="A16" s="15" t="s">
         <v>24</v>
       </c>
@@ -8013,7 +8415,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="34.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" ht="34.75" x14ac:dyDescent="0.4">
       <c r="A17" s="15" t="s">
         <v>27</v>
       </c>
@@ -8024,7 +8426,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="46" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" ht="46.3" x14ac:dyDescent="0.4">
       <c r="A18" s="15" t="s">
         <v>30</v>
       </c>
@@ -8035,7 +8437,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="46" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" ht="46.3" x14ac:dyDescent="0.4">
       <c r="A19" s="15" t="s">
         <v>33</v>
       </c>
@@ -8046,7 +8448,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="71" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" ht="69.45" x14ac:dyDescent="0.4">
       <c r="A20" s="18" t="s">
         <v>36</v>
       </c>

</xml_diff>

<commit_message>
reindexed economies of scale to 30 kW
</commit_message>
<xml_diff>
--- a/code/COSA_Data/historical_data.xlsx
+++ b/code/COSA_Data/historical_data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12163"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12170" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="annual_data" sheetId="1" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="137">
   <si>
     <t>source</t>
   </si>
@@ -444,6 +444,45 @@
   </si>
   <si>
     <t>Av bold</t>
+  </si>
+  <si>
+    <t>price_2019</t>
+  </si>
+  <si>
+    <t>CH_P_20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://iea-pvps.org/wp-content/uploads/2020/09/NSR_Switzerland_2019_v2.pdf </t>
+  </si>
+  <si>
+    <t>n_inst</t>
+  </si>
+  <si>
+    <t>2019 data</t>
+  </si>
+  <si>
+    <t>30-100</t>
+  </si>
+  <si>
+    <t>2-10</t>
+  </si>
+  <si>
+    <t>10-30</t>
+  </si>
+  <si>
+    <t>100-300</t>
+  </si>
+  <si>
+    <t>300-1000</t>
+  </si>
+  <si>
+    <t>&gt;1000</t>
+  </si>
+  <si>
+    <t>CHF/kWp</t>
+  </si>
+  <si>
+    <t>n_inst_model</t>
   </si>
 </sst>
 </file>
@@ -615,7 +654,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -697,6 +736,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="13" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -1285,7 +1325,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1472,11 +1511,23 @@
           <c:dPt>
             <c:idx val="10"/>
             <c:marker>
+              <c:symbol val="none"/>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-B69D-4695-A4A9-707898ACA78E}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="12"/>
+            <c:marker>
               <c:symbol val="circle"/>
               <c:size val="5"/>
               <c:spPr>
                 <a:solidFill>
-                  <a:sysClr val="window" lastClr="FFFFFF"/>
+                  <a:schemeClr val="bg1"/>
                 </a:solidFill>
                 <a:ln w="9525">
                   <a:solidFill>
@@ -1489,13 +1540,13 @@
             <c:bubble3D val="0"/>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000001-B69D-4695-A4A9-707898ACA78E}"/>
+                <c16:uniqueId val="{00000001-AFB6-4A7D-AF9A-9B93BF08D7BF}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
           <c:xVal>
             <c:numRef>
-              <c:f>scale_effect!$U$3:$U$21</c:f>
+              <c:f>scale_effect!$V$3:$V$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="19"/>
@@ -1561,66 +1612,66 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>scale_effect!$W$3:$W$21</c:f>
+              <c:f>scale_effect!$X$3:$X$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>2.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>2.4544829026085964</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0440338913330014</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>1.8365383433483464</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
+                  <c:v>1.7022218995608083</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.6048407008931183</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>1.5294246346336056</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.3741684991995822</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.2736677791107027</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.2008034274852089</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.144374231240699</c:v>
-                </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.0987379304981457</c:v>
+                  <c:v>1.4684329758879027</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.0606796665946323</c:v>
+                  <c:v>1.4175691546165046</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.0282056299187541</c:v>
+                  <c:v>1.3741684991995819</c:v>
                 </c:pt>
                 <c:pt idx="10">
+                  <c:v>1.3364724518267468</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.1129818763306365</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.83277577088054899</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.74823839326666097</c:v>
-                </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.69351548456569256</c:v>
+                  <c:v>0.92686434003732554</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.65384065180796802</c:v>
+                  <c:v>0.87384001902579322</c:v>
                 </c:pt>
                 <c:pt idx="15">
+                  <c:v>0.72771279547047851</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.60602158422756713</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>0.54450265284242116</c:v>
                 </c:pt>
-                <c:pt idx="16">
-                  <c:v>0.4534486164673513</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0.40741779009224771</c:v>
-                </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.35601796944565639</c:v>
+                  <c:v>0.47580820851941624</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1896,6 +1947,1159 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>2018</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>scale_effect!$V$4:$V$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>scale_effect!$W$4:$W$21</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>4702.1000000000004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3915.7949522574299</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3518.2917489791666</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3260.9791599763435</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3074.424128866247</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2929.9481234388008</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2813.1052323013746</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2715.6644337747043</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2632.5209652995222</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2560.3059239303489</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2132.1607394911325</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1915.7191907927581</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1775.6118034709691</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1674.032094130421</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1394.0933676682412</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1160.9671789393803</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1043.1141814877933</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>911.51491619736805</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-AD02-43D1-B985-A52FDE7D34C8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>2019</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>scale_effect!$V$4:$V$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>scale_effect!$U$4:$U$21</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>8399.4590139931479</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5128.4578258823367</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3898.2498283297709</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3237.8621696104556</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2821.3610714764895</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2532.9436383727425</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2320.5881659493721</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2157.2929721766232</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2027.5850524576672</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1921.9321546809817</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1421.0110464774064</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1242.7995012878118</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1151.6588389369954</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1096.7186686573955</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>989.94578636363121</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>945.9247163844293</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>937.37062624390796</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>937.56805909990817</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-AD02-43D1-B985-A52FDE7D34C8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>2018_median</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>scale_effect!$V$25:$V$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>scale_effect!$Z$25:$Z$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2953</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2214</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1589</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1236</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-AD02-43D1-B985-A52FDE7D34C8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>2019_median</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>scale_effect!$U$41:$U$46</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>scale_effect!$AA$41:$AA$46</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2914</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2201</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1466</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1217</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>990</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>777</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-AD02-43D1-B985-A52FDE7D34C8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="65065664"/>
+        <c:axId val="65066912"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="65065664"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="65066912"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="65066912"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="6000"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="65065664"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" b="1"/>
+              <a:t>Comparison n_inst in data</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" b="1" baseline="0"/>
+              <a:t> and in model</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" b="1"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>scale_effect!$V$41:$V$46</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2-10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10-30</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30-100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100-300</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>300-1000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>&gt;1000</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>scale_effect!$W$41:$W$46</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1043</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>711</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>187</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>117</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F0BF-444C-8ACC-85C6CA8EFD04}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>scale_effect!$V$41:$V$46</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2-10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10-30</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30-100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100-300</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>300-1000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>&gt;1000</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>scale_effect!$AE$41:$AE$46</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>928</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1828</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1862</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>216</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-F0BF-444C-8ACC-85C6CA8EFD04}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="2052506880"/>
+        <c:axId val="2052511872"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2052506880"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2052511872"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2052511872"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2052506880"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1976,6 +3180,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -2989,6 +4273,1025 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -3272,13 +5575,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>23</xdr:col>
+      <xdr:col>24</xdr:col>
       <xdr:colOff>120650</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>29</xdr:col>
+      <xdr:col>30</xdr:col>
       <xdr:colOff>63500</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
@@ -3327,7 +5630,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="de-CH" sz="1600" b="1"/>
-            <a:t>Scale effect (reference 10 kWp system):</a:t>
+            <a:t>Scale effect (reference 30 kWp system):</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -3337,7 +5640,7 @@
           </a:r>
           <a:r>
             <a:rPr lang="de-CH" sz="1600" baseline="0"/>
-            <a:t>_10 * Price_10 ^ Beta</a:t>
+            <a:t>_30 * Price_10 ^ Beta</a:t>
           </a:r>
           <a:endParaRPr lang="de-CH" sz="1600"/>
         </a:p>
@@ -3347,13 +5650,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>20</xdr:col>
+      <xdr:col>21</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>30</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
+      <xdr:col>27</xdr:col>
       <xdr:colOff>69850</xdr:colOff>
       <xdr:row>36</xdr:row>
       <xdr:rowOff>158750</xdr:rowOff>
@@ -3428,13 +5731,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>29</xdr:col>
+      <xdr:col>30</xdr:col>
       <xdr:colOff>238125</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>40</xdr:col>
+      <xdr:col>41</xdr:col>
       <xdr:colOff>12525</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>106275</xdr:rowOff>
@@ -3451,6 +5754,66 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>212912</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>78441</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>40</xdr:col>
+      <xdr:colOff>593910</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>179292</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>481853</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>118782</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>39</xdr:col>
+      <xdr:colOff>212912</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>4482</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="Chart 8"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3724,31 +6087,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BB49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AL1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="AL1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="AR54" sqref="AR54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="7.4609375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.07421875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.69140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.921875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.69140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.84375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.61328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.23046875" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="19.23046875" customWidth="1"/>
-    <col min="11" max="18" width="17.4609375" bestFit="1" customWidth="1"/>
-    <col min="19" max="24" width="17.23046875" bestFit="1" customWidth="1"/>
-    <col min="25" max="32" width="17.4609375" bestFit="1" customWidth="1"/>
-    <col min="33" max="38" width="17.23046875" bestFit="1" customWidth="1"/>
-    <col min="39" max="46" width="17.69140625" bestFit="1" customWidth="1"/>
-    <col min="47" max="52" width="17.53515625" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="17.3828125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.26953125" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="19.26953125" customWidth="1"/>
+    <col min="11" max="18" width="17.453125" bestFit="1" customWidth="1"/>
+    <col min="19" max="24" width="17.26953125" bestFit="1" customWidth="1"/>
+    <col min="25" max="32" width="17.453125" bestFit="1" customWidth="1"/>
+    <col min="33" max="38" width="17.26953125" bestFit="1" customWidth="1"/>
+    <col min="39" max="46" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="47" max="52" width="17.54296875" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="17.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:53" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3822,7 +6185,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="2" spans="1:53" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:53" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>71</v>
       </c>
@@ -3980,7 +6343,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="3" spans="1:53" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:53" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>44</v>
       </c>
@@ -4139,7 +6502,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:53" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:53" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -4300,7 +6663,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="5" spans="1:53" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:53" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>1991</v>
       </c>
@@ -4348,7 +6711,7 @@
       <c r="AK5" s="40"/>
       <c r="AL5" s="25"/>
     </row>
-    <row r="6" spans="1:53" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:53" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>1992</v>
       </c>
@@ -4396,7 +6759,7 @@
       <c r="AK6" s="40"/>
       <c r="AL6" s="25"/>
     </row>
-    <row r="7" spans="1:53" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:53" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>1993</v>
       </c>
@@ -4444,7 +6807,7 @@
       <c r="AK7" s="40"/>
       <c r="AL7" s="25"/>
     </row>
-    <row r="8" spans="1:53" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:53" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>1994</v>
       </c>
@@ -4492,7 +6855,7 @@
       <c r="AK8" s="40"/>
       <c r="AL8" s="25"/>
     </row>
-    <row r="9" spans="1:53" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:53" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>1995</v>
       </c>
@@ -4540,7 +6903,7 @@
       <c r="AK9" s="40"/>
       <c r="AL9" s="25"/>
     </row>
-    <row r="10" spans="1:53" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:53" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>1996</v>
       </c>
@@ -4588,7 +6951,7 @@
       <c r="AK10" s="40"/>
       <c r="AL10" s="25"/>
     </row>
-    <row r="11" spans="1:53" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:53" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>1997</v>
       </c>
@@ -4636,7 +6999,7 @@
       <c r="AK11" s="40"/>
       <c r="AL11" s="25"/>
     </row>
-    <row r="12" spans="1:53" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:53" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>1998</v>
       </c>
@@ -4684,7 +7047,7 @@
       <c r="AK12" s="40"/>
       <c r="AL12" s="25"/>
     </row>
-    <row r="13" spans="1:53" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:53" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>1999</v>
       </c>
@@ -4732,7 +7095,7 @@
       <c r="AK13" s="40"/>
       <c r="AL13" s="25"/>
     </row>
-    <row r="14" spans="1:53" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:53" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>2000</v>
       </c>
@@ -4780,7 +7143,7 @@
       <c r="AK14" s="40"/>
       <c r="AL14" s="25"/>
     </row>
-    <row r="15" spans="1:53" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:53" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>2001</v>
       </c>
@@ -4828,7 +7191,7 @@
       <c r="AK15" s="40"/>
       <c r="AL15" s="25"/>
     </row>
-    <row r="16" spans="1:53" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:53" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>2002</v>
       </c>
@@ -4876,7 +7239,7 @@
       <c r="AK16" s="40"/>
       <c r="AL16" s="25"/>
     </row>
-    <row r="17" spans="1:53" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:53" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>2003</v>
       </c>
@@ -4924,7 +7287,7 @@
       <c r="AK17" s="40"/>
       <c r="AL17" s="25"/>
     </row>
-    <row r="18" spans="1:53" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:53" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>2004</v>
       </c>
@@ -4972,7 +7335,7 @@
       <c r="AK18" s="40"/>
       <c r="AL18" s="25"/>
     </row>
-    <row r="19" spans="1:53" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:53" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>2005</v>
       </c>
@@ -5020,7 +7383,7 @@
       <c r="AK19" s="40"/>
       <c r="AL19" s="25"/>
     </row>
-    <row r="20" spans="1:53" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:53" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>2006</v>
       </c>
@@ -5068,7 +7431,7 @@
       <c r="AK20" s="40"/>
       <c r="AL20" s="25"/>
     </row>
-    <row r="21" spans="1:53" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:53" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>2007</v>
       </c>
@@ -5116,7 +7479,7 @@
       <c r="AK21" s="40"/>
       <c r="AL21" s="25"/>
     </row>
-    <row r="22" spans="1:53" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:53" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>2008</v>
       </c>
@@ -5164,7 +7527,7 @@
       <c r="AK22" s="40"/>
       <c r="AL22" s="25"/>
     </row>
-    <row r="23" spans="1:53" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:53" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>2009</v>
       </c>
@@ -5344,7 +7707,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="24" spans="1:53" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:53" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>2010</v>
       </c>
@@ -5524,7 +7887,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:53" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:53" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>2011</v>
       </c>
@@ -5704,7 +8067,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:53" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:53" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <v>2012</v>
       </c>
@@ -5884,7 +8247,7 @@
         <v>8.8191039627855516E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:53" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:53" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>2013</v>
       </c>
@@ -6064,7 +8427,7 @@
         <v>0.14070792426841286</v>
       </c>
     </row>
-    <row r="28" spans="1:53" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:53" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>2014</v>
       </c>
@@ -6245,7 +8608,7 @@
         <v>2.9767482187529257E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:53" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:53" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <v>2015</v>
       </c>
@@ -6426,7 +8789,7 @@
         <v>0.20373744217920156</v>
       </c>
     </row>
-    <row r="30" spans="1:53" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:53" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <v>2016</v>
       </c>
@@ -6607,7 +8970,7 @@
         <v>6.9797836069996691E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:53" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:53" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
         <v>2017</v>
       </c>
@@ -6793,7 +9156,7 @@
         <v>9.3553539982954119E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:53" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:53" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
         <v>2018</v>
       </c>
@@ -6970,7 +9333,7 @@
         <v>4.8423454763032048E-3</v>
       </c>
       <c r="AY32">
-        <f t="shared" ref="AY23:AY34" si="30">(W32-W31)/W31</f>
+        <f t="shared" ref="AY32:AY34" si="30">(W32-W31)/W31</f>
         <v>2.9148583955975142E-2</v>
       </c>
       <c r="AZ32">
@@ -6982,7 +9345,7 @@
         <v>1.6852375794482774E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:54" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:54" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A33" s="1">
         <v>2019</v>
       </c>
@@ -7164,7 +9527,7 @@
         <v>-8.6828999057985794E-3</v>
       </c>
     </row>
-    <row r="34" spans="1:54" s="33" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:54" s="33" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A34" s="32">
         <v>2020</v>
       </c>
@@ -7331,7 +9694,7 @@
         <v>-2.0677036126294537E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:54" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:54" x14ac:dyDescent="0.35">
       <c r="A35" s="1">
         <v>2021</v>
       </c>
@@ -7340,7 +9703,7 @@
         <v>1.9272329300234889</v>
       </c>
     </row>
-    <row r="36" spans="1:54" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:54" x14ac:dyDescent="0.35">
       <c r="A36" s="1">
         <v>2022</v>
       </c>
@@ -7349,7 +9712,7 @@
         <v>1.8104018908676494</v>
       </c>
     </row>
-    <row r="37" spans="1:54" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:54" x14ac:dyDescent="0.35">
       <c r="A37" s="1">
         <v>2023</v>
       </c>
@@ -7364,7 +9727,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="38" spans="1:54" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:54" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A38" s="1">
         <v>2024</v>
       </c>
@@ -7440,7 +9803,7 @@
         <v>5.6642863506644089E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:54" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:54" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A39" s="1">
         <v>2025</v>
       </c>
@@ -7516,7 +9879,7 @@
         <v>3.1120205186508415E-3</v>
       </c>
     </row>
-    <row r="40" spans="1:54" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:54" x14ac:dyDescent="0.35">
       <c r="A40" s="1">
         <v>2026</v>
       </c>
@@ -7532,7 +9895,7 @@
         <v>1.1477207120931338E-2</v>
       </c>
       <c r="AN40" s="38">
-        <f t="shared" ref="AN40:BA40" si="35">AVERAGE(AN30:AN34)</f>
+        <f t="shared" ref="AN40:AZ40" si="35">AVERAGE(AN30:AN34)</f>
         <v>1.1978953630635185E-2</v>
       </c>
       <c r="AO40" s="22">
@@ -7592,7 +9955,7 @@
         <v>1.2493825957213352E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:54" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:54" x14ac:dyDescent="0.35">
       <c r="A41" s="1">
         <v>2027</v>
       </c>
@@ -7608,7 +9971,7 @@
         <v>-1.3220964188851509E-2</v>
       </c>
       <c r="AN41" s="38">
-        <f t="shared" ref="AN41:BA41" si="37">AVERAGE(AN33:AN34)</f>
+        <f t="shared" ref="AN41:AZ41" si="37">AVERAGE(AN33:AN34)</f>
         <v>-1.3358765644955757E-2</v>
       </c>
       <c r="AO41" s="22">
@@ -7668,7 +10031,7 @@
         <v>-1.4556991457375774E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:54" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:54" x14ac:dyDescent="0.35">
       <c r="A42" s="1">
         <v>2028</v>
       </c>
@@ -7677,7 +10040,7 @@
         <v>1.2439980957732839</v>
       </c>
     </row>
-    <row r="43" spans="1:54" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:54" x14ac:dyDescent="0.35">
       <c r="A43" s="1">
         <v>2029</v>
       </c>
@@ -7686,7 +10049,7 @@
         <v>1.1685855247379255</v>
       </c>
     </row>
-    <row r="44" spans="1:54" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:54" x14ac:dyDescent="0.35">
       <c r="A44" s="1">
         <v>2030</v>
       </c>
@@ -7695,7 +10058,7 @@
         <v>1.0977445490205067</v>
       </c>
     </row>
-    <row r="45" spans="1:54" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:54" x14ac:dyDescent="0.35">
       <c r="A45" s="1">
         <v>2031</v>
       </c>
@@ -7704,7 +10067,7 @@
         <v>1.0311980333441888</v>
       </c>
     </row>
-    <row r="46" spans="1:54" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:54" x14ac:dyDescent="0.35">
       <c r="A46" s="1">
         <v>2032</v>
       </c>
@@ -7713,7 +10076,7 @@
         <v>0.96868564268594526</v>
       </c>
     </row>
-    <row r="47" spans="1:54" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:54" x14ac:dyDescent="0.35">
       <c r="A47" s="1">
         <v>2033</v>
       </c>
@@ -7722,7 +10085,7 @@
         <v>0.90996282382618143</v>
       </c>
     </row>
-    <row r="48" spans="1:54" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:54" x14ac:dyDescent="0.35">
       <c r="A48" s="1">
         <v>2034</v>
       </c>
@@ -7731,7 +10094,7 @@
         <v>0.85479984863796732</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" s="1">
         <v>2035</v>
       </c>
@@ -7765,509 +10128,874 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:AC29"/>
+  <dimension ref="B1:AE46"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F44" sqref="F44"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AC12" sqref="AC12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="21" max="21" width="10.7265625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="2:26" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:27" x14ac:dyDescent="0.35">
+      <c r="U1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="2" spans="2:27" x14ac:dyDescent="0.35">
       <c r="B2" s="19" t="s">
         <v>49</v>
       </c>
       <c r="U2" t="s">
+        <v>124</v>
+      </c>
+      <c r="V2" t="s">
         <v>53</v>
       </c>
-      <c r="V2" t="s">
+      <c r="W2" t="s">
         <v>54</v>
       </c>
-      <c r="W2" s="1" t="s">
+      <c r="X2" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Y2" t="s">
         <v>57</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="Z2" t="s">
         <v>55</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AA2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="2:26" x14ac:dyDescent="0.4">
-      <c r="U3">
+    <row r="3" spans="2:27" x14ac:dyDescent="0.35">
+      <c r="U3" s="7" t="e">
+        <f>8120/(V3^0.766)+1140*EXP(-2.99*10^-4 *W3)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V3">
         <v>0</v>
       </c>
-      <c r="V3" s="7" t="e">
-        <f>$Y$3*U3^$Z$3</f>
+      <c r="W3" s="7" t="e">
+        <f>$Z$3*V3^$AA$3</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="W3">
+      <c r="X3">
+        <v>2.5</v>
+      </c>
+      <c r="Y3">
+        <v>1</v>
+      </c>
+      <c r="Z3">
+        <v>4702.1000000000004</v>
+      </c>
+      <c r="AA3" s="8">
+        <v>-0.26400000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="2:27" x14ac:dyDescent="0.35">
+      <c r="U4" s="7">
+        <f t="shared" ref="U4:U21" si="0">8120/(V4^0.766)+1140*EXP(-2.99*10^-4 *W4)</f>
+        <v>8399.4590139931479</v>
+      </c>
+      <c r="V4">
+        <v>1</v>
+      </c>
+      <c r="W4" s="7">
+        <f t="shared" ref="W4:W21" si="1">$Z$3*V4^$AA$3</f>
+        <v>4702.1000000000004</v>
+      </c>
+      <c r="X4">
+        <f>$Z$4*V4^$AA$3</f>
+        <v>2.4544829026085964</v>
+      </c>
+      <c r="Y4">
+        <v>30</v>
+      </c>
+      <c r="Z4">
+        <f>Z3/VLOOKUP(Y4,$V$3:$W$21,2,0)</f>
+        <v>2.4544829026085964</v>
+      </c>
+      <c r="AA4" s="8">
+        <f>AA3</f>
+        <v>-0.26400000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="2:27" x14ac:dyDescent="0.35">
+      <c r="U5" s="7">
+        <f t="shared" si="0"/>
+        <v>5128.4578258823367</v>
+      </c>
+      <c r="V5">
         <v>2</v>
       </c>
-      <c r="X3">
+      <c r="W5" s="7">
+        <f t="shared" si="1"/>
+        <v>3915.7949522574299</v>
+      </c>
+      <c r="X5">
+        <f t="shared" ref="X5:X21" si="2">$Z$4*V5^$AA$3</f>
+        <v>2.0440338913330014</v>
+      </c>
+    </row>
+    <row r="6" spans="2:27" x14ac:dyDescent="0.35">
+      <c r="U6" s="7">
+        <f t="shared" si="0"/>
+        <v>3898.2498283297709</v>
+      </c>
+      <c r="V6">
+        <v>3</v>
+      </c>
+      <c r="W6" s="7">
+        <f t="shared" si="1"/>
+        <v>3518.2917489791666</v>
+      </c>
+      <c r="X6">
+        <f t="shared" si="2"/>
+        <v>1.8365383433483464</v>
+      </c>
+    </row>
+    <row r="7" spans="2:27" x14ac:dyDescent="0.35">
+      <c r="U7" s="7">
+        <f t="shared" si="0"/>
+        <v>3237.8621696104556</v>
+      </c>
+      <c r="V7">
+        <v>4</v>
+      </c>
+      <c r="W7" s="7">
+        <f t="shared" si="1"/>
+        <v>3260.9791599763435</v>
+      </c>
+      <c r="X7">
+        <f t="shared" si="2"/>
+        <v>1.7022218995608083</v>
+      </c>
+    </row>
+    <row r="8" spans="2:27" x14ac:dyDescent="0.35">
+      <c r="U8" s="7">
+        <f t="shared" si="0"/>
+        <v>2821.3610714764895</v>
+      </c>
+      <c r="V8">
+        <v>5</v>
+      </c>
+      <c r="W8" s="7">
+        <f t="shared" si="1"/>
+        <v>3074.424128866247</v>
+      </c>
+      <c r="X8">
+        <f t="shared" si="2"/>
+        <v>1.6048407008931183</v>
+      </c>
+    </row>
+    <row r="9" spans="2:27" x14ac:dyDescent="0.35">
+      <c r="U9" s="7">
+        <f t="shared" si="0"/>
+        <v>2532.9436383727425</v>
+      </c>
+      <c r="V9">
+        <v>6</v>
+      </c>
+      <c r="W9" s="7">
+        <f t="shared" si="1"/>
+        <v>2929.9481234388008</v>
+      </c>
+      <c r="X9">
+        <f t="shared" si="2"/>
+        <v>1.5294246346336056</v>
+      </c>
+    </row>
+    <row r="10" spans="2:27" x14ac:dyDescent="0.35">
+      <c r="U10" s="7">
+        <f t="shared" si="0"/>
+        <v>2320.5881659493721</v>
+      </c>
+      <c r="V10">
+        <v>7</v>
+      </c>
+      <c r="W10" s="7">
+        <f t="shared" si="1"/>
+        <v>2813.1052323013746</v>
+      </c>
+      <c r="X10">
+        <f t="shared" si="2"/>
+        <v>1.4684329758879027</v>
+      </c>
+    </row>
+    <row r="11" spans="2:27" x14ac:dyDescent="0.35">
+      <c r="U11" s="7">
+        <f t="shared" si="0"/>
+        <v>2157.2929721766232</v>
+      </c>
+      <c r="V11">
+        <v>8</v>
+      </c>
+      <c r="W11" s="7">
+        <f t="shared" si="1"/>
+        <v>2715.6644337747043</v>
+      </c>
+      <c r="X11">
+        <f t="shared" si="2"/>
+        <v>1.4175691546165046</v>
+      </c>
+    </row>
+    <row r="12" spans="2:27" x14ac:dyDescent="0.35">
+      <c r="U12" s="7">
+        <f t="shared" si="0"/>
+        <v>2027.5850524576672</v>
+      </c>
+      <c r="V12">
+        <v>9</v>
+      </c>
+      <c r="W12" s="7">
+        <f t="shared" si="1"/>
+        <v>2632.5209652995222</v>
+      </c>
+      <c r="X12">
+        <f t="shared" si="2"/>
+        <v>1.3741684991995819</v>
+      </c>
+    </row>
+    <row r="13" spans="2:27" x14ac:dyDescent="0.35">
+      <c r="U13" s="7">
+        <f t="shared" si="0"/>
+        <v>1921.9321546809817</v>
+      </c>
+      <c r="V13">
+        <v>10</v>
+      </c>
+      <c r="W13" s="7">
+        <f t="shared" si="1"/>
+        <v>2560.3059239303489</v>
+      </c>
+      <c r="X13">
+        <f t="shared" si="2"/>
+        <v>1.3364724518267468</v>
+      </c>
+    </row>
+    <row r="14" spans="2:27" x14ac:dyDescent="0.35">
+      <c r="U14" s="7">
+        <f t="shared" si="0"/>
+        <v>1421.0110464774064</v>
+      </c>
+      <c r="V14">
+        <v>20</v>
+      </c>
+      <c r="W14" s="7">
+        <f t="shared" si="1"/>
+        <v>2132.1607394911325</v>
+      </c>
+      <c r="X14">
+        <f t="shared" si="2"/>
+        <v>1.1129818763306365</v>
+      </c>
+    </row>
+    <row r="15" spans="2:27" x14ac:dyDescent="0.35">
+      <c r="U15" s="7">
+        <f t="shared" si="0"/>
+        <v>1242.7995012878118</v>
+      </c>
+      <c r="V15">
+        <v>30</v>
+      </c>
+      <c r="W15" s="7">
+        <f t="shared" si="1"/>
+        <v>1915.7191907927581</v>
+      </c>
+      <c r="X15">
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="Y3">
-        <v>4702.1000000000004</v>
-      </c>
-      <c r="Z3" s="8">
-        <v>-0.26400000000000001</v>
-      </c>
     </row>
-    <row r="4" spans="2:26" x14ac:dyDescent="0.4">
-      <c r="U4">
-        <v>1</v>
-      </c>
-      <c r="V4" s="7">
-        <f t="shared" ref="V4:V21" si="0">$Y$3*U4^$Z$3</f>
-        <v>4702.1000000000004</v>
-      </c>
-      <c r="W4">
-        <f>$Y$4*U4^$Z$3</f>
-        <v>1.8365383433483464</v>
-      </c>
-      <c r="X4">
-        <v>10</v>
-      </c>
-      <c r="Y4">
-        <f>Y3/V13</f>
-        <v>1.8365383433483464</v>
-      </c>
-      <c r="Z4" s="8">
-        <f>Z3</f>
-        <v>-0.26400000000000001</v>
+    <row r="16" spans="2:27" x14ac:dyDescent="0.35">
+      <c r="U16" s="7">
+        <f t="shared" si="0"/>
+        <v>1151.6588389369954</v>
+      </c>
+      <c r="V16">
+        <v>40</v>
+      </c>
+      <c r="W16" s="7">
+        <f t="shared" si="1"/>
+        <v>1775.6118034709691</v>
+      </c>
+      <c r="X16">
+        <f t="shared" si="2"/>
+        <v>0.92686434003732554</v>
       </c>
     </row>
-    <row r="5" spans="2:26" x14ac:dyDescent="0.4">
-      <c r="U5">
-        <v>2</v>
-      </c>
-      <c r="V5" s="7">
+    <row r="17" spans="21:30" x14ac:dyDescent="0.35">
+      <c r="U17" s="7">
         <f t="shared" si="0"/>
-        <v>3915.7949522574299</v>
-      </c>
-      <c r="W5">
-        <f t="shared" ref="W5:W21" si="1">$Y$4*U5^$Z$3</f>
-        <v>1.5294246346336056</v>
+        <v>1096.7186686573955</v>
+      </c>
+      <c r="V17">
+        <v>50</v>
+      </c>
+      <c r="W17" s="7">
+        <f t="shared" si="1"/>
+        <v>1674.032094130421</v>
+      </c>
+      <c r="X17">
+        <f t="shared" si="2"/>
+        <v>0.87384001902579322</v>
       </c>
     </row>
-    <row r="6" spans="2:26" x14ac:dyDescent="0.4">
-      <c r="U6">
-        <v>3</v>
-      </c>
-      <c r="V6" s="7">
+    <row r="18" spans="21:30" x14ac:dyDescent="0.35">
+      <c r="U18" s="7">
         <f t="shared" si="0"/>
-        <v>3518.2917489791666</v>
-      </c>
-      <c r="W6">
+        <v>989.94578636363121</v>
+      </c>
+      <c r="V18">
+        <v>100</v>
+      </c>
+      <c r="W18" s="7">
         <f t="shared" si="1"/>
-        <v>1.3741684991995822</v>
+        <v>1394.0933676682412</v>
+      </c>
+      <c r="X18">
+        <f t="shared" si="2"/>
+        <v>0.72771279547047851</v>
       </c>
     </row>
-    <row r="7" spans="2:26" x14ac:dyDescent="0.4">
-      <c r="U7">
-        <v>4</v>
-      </c>
-      <c r="V7" s="7">
+    <row r="19" spans="21:30" x14ac:dyDescent="0.35">
+      <c r="U19" s="7">
         <f t="shared" si="0"/>
-        <v>3260.9791599763435</v>
-      </c>
-      <c r="W7">
+        <v>945.9247163844293</v>
+      </c>
+      <c r="V19">
+        <v>200</v>
+      </c>
+      <c r="W19" s="7">
         <f t="shared" si="1"/>
-        <v>1.2736677791107027</v>
+        <v>1160.9671789393803</v>
+      </c>
+      <c r="X19">
+        <f t="shared" si="2"/>
+        <v>0.60602158422756713</v>
       </c>
     </row>
-    <row r="8" spans="2:26" x14ac:dyDescent="0.4">
-      <c r="U8">
-        <v>5</v>
-      </c>
-      <c r="V8" s="7">
+    <row r="20" spans="21:30" x14ac:dyDescent="0.35">
+      <c r="U20" s="7">
         <f t="shared" si="0"/>
-        <v>3074.424128866247</v>
-      </c>
-      <c r="W8">
+        <v>937.37062624390796</v>
+      </c>
+      <c r="V20">
+        <v>300</v>
+      </c>
+      <c r="W20" s="7">
         <f t="shared" si="1"/>
-        <v>1.2008034274852089</v>
+        <v>1043.1141814877933</v>
+      </c>
+      <c r="X20">
+        <f t="shared" si="2"/>
+        <v>0.54450265284242116</v>
       </c>
     </row>
-    <row r="9" spans="2:26" x14ac:dyDescent="0.4">
-      <c r="U9">
-        <v>6</v>
-      </c>
-      <c r="V9" s="7">
+    <row r="21" spans="21:30" x14ac:dyDescent="0.35">
+      <c r="U21" s="7">
         <f t="shared" si="0"/>
-        <v>2929.9481234388008</v>
-      </c>
-      <c r="W9">
+        <v>937.56805909990817</v>
+      </c>
+      <c r="V21">
+        <v>500</v>
+      </c>
+      <c r="W21" s="7">
         <f t="shared" si="1"/>
-        <v>1.144374231240699</v>
+        <v>911.51491619736805</v>
+      </c>
+      <c r="X21">
+        <f t="shared" si="2"/>
+        <v>0.47580820851941624</v>
       </c>
     </row>
-    <row r="10" spans="2:26" x14ac:dyDescent="0.4">
-      <c r="U10">
-        <v>7</v>
-      </c>
-      <c r="V10" s="7">
-        <f t="shared" si="0"/>
-        <v>2813.1052323013746</v>
-      </c>
-      <c r="W10">
-        <f t="shared" si="1"/>
-        <v>1.0987379304981457</v>
-      </c>
+    <row r="22" spans="21:30" x14ac:dyDescent="0.35">
+      <c r="W22" s="7"/>
     </row>
-    <row r="11" spans="2:26" x14ac:dyDescent="0.4">
-      <c r="U11">
-        <v>8</v>
-      </c>
-      <c r="V11" s="7">
-        <f t="shared" si="0"/>
-        <v>2715.6644337747043</v>
-      </c>
-      <c r="W11">
-        <f t="shared" si="1"/>
-        <v>1.0606796665946323</v>
-      </c>
-    </row>
-    <row r="12" spans="2:26" x14ac:dyDescent="0.4">
-      <c r="U12">
-        <v>9</v>
-      </c>
-      <c r="V12" s="7">
-        <f t="shared" si="0"/>
-        <v>2632.5209652995222</v>
-      </c>
-      <c r="W12">
-        <f t="shared" si="1"/>
-        <v>1.0282056299187541</v>
-      </c>
-    </row>
-    <row r="13" spans="2:26" x14ac:dyDescent="0.4">
-      <c r="U13">
-        <v>10</v>
-      </c>
-      <c r="V13" s="7">
-        <f t="shared" si="0"/>
-        <v>2560.3059239303489</v>
-      </c>
-      <c r="W13">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="2:26" x14ac:dyDescent="0.4">
-      <c r="U14">
-        <v>20</v>
-      </c>
-      <c r="V14" s="7">
-        <f t="shared" si="0"/>
-        <v>2132.1607394911325</v>
-      </c>
-      <c r="W14">
-        <f t="shared" si="1"/>
-        <v>0.83277577088054899</v>
-      </c>
-    </row>
-    <row r="15" spans="2:26" x14ac:dyDescent="0.4">
-      <c r="U15">
-        <v>30</v>
-      </c>
-      <c r="V15" s="7">
-        <f t="shared" si="0"/>
-        <v>1915.7191907927581</v>
-      </c>
-      <c r="W15">
-        <f t="shared" si="1"/>
-        <v>0.74823839326666097</v>
-      </c>
-    </row>
-    <row r="16" spans="2:26" x14ac:dyDescent="0.4">
-      <c r="U16">
-        <v>40</v>
-      </c>
-      <c r="V16" s="7">
-        <f t="shared" si="0"/>
-        <v>1775.6118034709691</v>
-      </c>
-      <c r="W16">
-        <f t="shared" si="1"/>
-        <v>0.69351548456569256</v>
-      </c>
-    </row>
-    <row r="17" spans="21:29" x14ac:dyDescent="0.4">
-      <c r="U17">
-        <v>50</v>
-      </c>
-      <c r="V17" s="7">
-        <f t="shared" si="0"/>
-        <v>1674.032094130421</v>
-      </c>
-      <c r="W17">
-        <f t="shared" si="1"/>
-        <v>0.65384065180796802</v>
-      </c>
-    </row>
-    <row r="18" spans="21:29" x14ac:dyDescent="0.4">
-      <c r="U18">
-        <v>100</v>
-      </c>
-      <c r="V18" s="7">
-        <f t="shared" si="0"/>
-        <v>1394.0933676682412</v>
-      </c>
-      <c r="W18">
-        <f t="shared" si="1"/>
-        <v>0.54450265284242116</v>
-      </c>
-    </row>
-    <row r="19" spans="21:29" x14ac:dyDescent="0.4">
-      <c r="U19">
-        <v>200</v>
-      </c>
-      <c r="V19" s="7">
-        <f t="shared" si="0"/>
-        <v>1160.9671789393803</v>
-      </c>
-      <c r="W19">
-        <f t="shared" si="1"/>
-        <v>0.4534486164673513</v>
-      </c>
-    </row>
-    <row r="20" spans="21:29" x14ac:dyDescent="0.4">
-      <c r="U20">
-        <v>300</v>
-      </c>
-      <c r="V20" s="7">
-        <f t="shared" si="0"/>
-        <v>1043.1141814877933</v>
-      </c>
-      <c r="W20">
-        <f t="shared" si="1"/>
-        <v>0.40741779009224771</v>
-      </c>
-    </row>
-    <row r="21" spans="21:29" x14ac:dyDescent="0.4">
-      <c r="U21">
-        <v>500</v>
-      </c>
-      <c r="V21" s="7">
-        <f t="shared" si="0"/>
-        <v>911.51491619736805</v>
-      </c>
-      <c r="W21">
-        <f t="shared" si="1"/>
-        <v>0.35601796944565639</v>
-      </c>
-    </row>
-    <row r="22" spans="21:29" x14ac:dyDescent="0.4">
-      <c r="V22" s="7"/>
-    </row>
-    <row r="23" spans="21:29" x14ac:dyDescent="0.4">
-      <c r="AA23" t="s">
+    <row r="23" spans="21:30" x14ac:dyDescent="0.35">
+      <c r="AB23" t="s">
         <v>69</v>
-      </c>
-      <c r="AB23" s="21">
-        <f>AVERAGE(AB25:AB29)</f>
-        <v>0.57139832352176323</v>
       </c>
       <c r="AC23" s="21">
         <f>AVERAGE(AC25:AC29)</f>
+        <v>0.57139832352176323</v>
+      </c>
+      <c r="AD23" s="21">
+        <f>AVERAGE(AD25:AD29)</f>
         <v>1.986667714406829</v>
       </c>
     </row>
-    <row r="24" spans="21:29" x14ac:dyDescent="0.4">
-      <c r="U24" t="s">
+    <row r="24" spans="21:30" x14ac:dyDescent="0.35">
+      <c r="V24" t="s">
         <v>58</v>
       </c>
-      <c r="V24" t="s">
+      <c r="W24" t="s">
         <v>60</v>
       </c>
-      <c r="W24" t="s">
+      <c r="X24" t="s">
         <v>61</v>
       </c>
-      <c r="X24" t="s">
+      <c r="Y24" t="s">
         <v>62</v>
       </c>
-      <c r="Y24" t="s">
+      <c r="Z24" t="s">
         <v>63</v>
       </c>
-      <c r="Z24" t="s">
+      <c r="AA24" t="s">
         <v>64</v>
       </c>
-      <c r="AA24" t="s">
+      <c r="AB24" t="s">
         <v>65</v>
       </c>
-      <c r="AB24" t="s">
+      <c r="AC24" t="s">
         <v>67</v>
       </c>
-      <c r="AC24" t="s">
+      <c r="AD24" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="25" spans="21:29" x14ac:dyDescent="0.4">
-      <c r="U25">
+    <row r="25" spans="21:30" x14ac:dyDescent="0.35">
+      <c r="V25">
         <v>2</v>
       </c>
-      <c r="V25">
+      <c r="W25">
         <v>2956</v>
       </c>
-      <c r="W25">
+      <c r="X25">
         <v>1558</v>
       </c>
-      <c r="X25">
+      <c r="Y25">
         <v>2581</v>
       </c>
-      <c r="Y25">
+      <c r="Z25">
         <v>2953</v>
       </c>
-      <c r="Z25">
+      <c r="AA25">
         <v>3402</v>
       </c>
-      <c r="AA25">
+      <c r="AB25">
         <v>5698</v>
       </c>
-      <c r="AB25" s="7">
-        <f>W25/Y25</f>
+      <c r="AC25" s="7">
+        <f>X25/Z25</f>
         <v>0.52759905181171685</v>
       </c>
-      <c r="AC25">
-        <f>AA25/Y25</f>
+      <c r="AD25">
+        <f>AB25/Z25</f>
         <v>1.929563156112428</v>
       </c>
     </row>
-    <row r="26" spans="21:29" x14ac:dyDescent="0.4">
-      <c r="U26">
+    <row r="26" spans="21:30" x14ac:dyDescent="0.35">
+      <c r="V26">
         <v>10</v>
       </c>
-      <c r="V26">
+      <c r="W26">
         <v>2219</v>
       </c>
-      <c r="W26">
+      <c r="X26">
         <v>1070</v>
       </c>
-      <c r="X26">
+      <c r="Y26">
         <v>1994</v>
       </c>
-      <c r="Y26">
+      <c r="Z26">
         <v>2214</v>
       </c>
-      <c r="Z26">
+      <c r="AA26">
         <v>2574</v>
       </c>
-      <c r="AA26">
+      <c r="AB26">
         <v>4684</v>
       </c>
-      <c r="AB26" s="21">
-        <f t="shared" ref="AB26:AB29" si="2">W26/Y26</f>
+      <c r="AC26" s="21">
+        <f t="shared" ref="AC26:AC29" si="3">X26/Z26</f>
         <v>0.48328816621499548</v>
       </c>
-      <c r="AC26" s="1">
-        <f t="shared" ref="AC26:AC29" si="3">AA26/Y26</f>
+      <c r="AD26" s="1">
+        <f t="shared" ref="AD26:AD29" si="4">AB26/Z26</f>
         <v>2.1156278229448962</v>
       </c>
     </row>
-    <row r="27" spans="21:29" x14ac:dyDescent="0.4">
-      <c r="U27">
+    <row r="27" spans="21:30" x14ac:dyDescent="0.35">
+      <c r="V27">
         <v>30</v>
       </c>
-      <c r="V27">
+      <c r="W27">
         <v>1595</v>
       </c>
-      <c r="W27">
+      <c r="X27">
         <v>817</v>
       </c>
-      <c r="X27">
+      <c r="Y27">
         <v>1377</v>
       </c>
-      <c r="Y27">
+      <c r="Z27">
         <v>1589</v>
       </c>
-      <c r="Z27">
+      <c r="AA27">
         <v>1787</v>
       </c>
-      <c r="AA27">
+      <c r="AB27">
         <v>3500</v>
       </c>
-      <c r="AB27" s="7">
-        <f t="shared" si="2"/>
+      <c r="AC27" s="7">
+        <f t="shared" si="3"/>
         <v>0.51415984896161104</v>
       </c>
-      <c r="AC27">
+      <c r="AD27">
+        <f t="shared" si="4"/>
+        <v>2.2026431718061672</v>
+      </c>
+    </row>
+    <row r="28" spans="21:30" x14ac:dyDescent="0.35">
+      <c r="V28">
+        <v>100</v>
+      </c>
+      <c r="W28">
+        <v>1296</v>
+      </c>
+      <c r="X28">
+        <v>875</v>
+      </c>
+      <c r="Y28">
+        <v>1130</v>
+      </c>
+      <c r="Z28">
+        <v>1236</v>
+      </c>
+      <c r="AA28">
+        <v>1398</v>
+      </c>
+      <c r="AB28">
+        <v>2857</v>
+      </c>
+      <c r="AC28" s="7">
         <f t="shared" si="3"/>
-        <v>2.2026431718061672</v>
+        <v>0.70792880258899671</v>
+      </c>
+      <c r="AD28">
+        <f t="shared" si="4"/>
+        <v>2.3114886731391584</v>
       </c>
     </row>
-    <row r="28" spans="21:29" x14ac:dyDescent="0.4">
-      <c r="U28">
+    <row r="29" spans="21:30" x14ac:dyDescent="0.35">
+      <c r="V29" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="W29">
+        <v>1000</v>
+      </c>
+      <c r="X29">
+        <v>634</v>
+      </c>
+      <c r="Y29">
+        <v>927</v>
+      </c>
+      <c r="Z29">
+        <v>1016</v>
+      </c>
+      <c r="AA29">
+        <v>1165</v>
+      </c>
+      <c r="AB29">
+        <v>1396</v>
+      </c>
+      <c r="AC29" s="7">
+        <f t="shared" si="3"/>
+        <v>0.62401574803149606</v>
+      </c>
+      <c r="AD29">
+        <f t="shared" si="4"/>
+        <v>1.3740157480314961</v>
+      </c>
+    </row>
+    <row r="39" spans="21:31" x14ac:dyDescent="0.35">
+      <c r="V39" t="s">
+        <v>128</v>
+      </c>
+      <c r="X39" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="40" spans="21:31" x14ac:dyDescent="0.35">
+      <c r="V40" t="s">
+        <v>58</v>
+      </c>
+      <c r="W40" t="s">
+        <v>127</v>
+      </c>
+      <c r="X40" t="s">
+        <v>69</v>
+      </c>
+      <c r="Y40" t="s">
+        <v>61</v>
+      </c>
+      <c r="Z40" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA40" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB40" t="s">
+        <v>64</v>
+      </c>
+      <c r="AC40" t="s">
+        <v>65</v>
+      </c>
+      <c r="AE40" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="41" spans="21:31" x14ac:dyDescent="0.35">
+      <c r="U41">
+        <v>2</v>
+      </c>
+      <c r="V41" s="47" t="s">
+        <v>130</v>
+      </c>
+      <c r="W41">
+        <v>1043</v>
+      </c>
+      <c r="X41">
+        <v>2985</v>
+      </c>
+      <c r="Y41">
+        <v>1359</v>
+      </c>
+      <c r="Z41">
+        <v>2538</v>
+      </c>
+      <c r="AA41">
+        <v>2914</v>
+      </c>
+      <c r="AB41">
+        <v>3528</v>
+      </c>
+      <c r="AC41">
+        <v>7545</v>
+      </c>
+      <c r="AD41" s="7">
+        <f t="shared" ref="AD41:AD46" si="5">AA41/$AA$42</f>
+        <v>1.323943661971831</v>
+      </c>
+      <c r="AE41">
+        <v>928</v>
+      </c>
+    </row>
+    <row r="42" spans="21:31" x14ac:dyDescent="0.35">
+      <c r="U42">
+        <v>10</v>
+      </c>
+      <c r="V42" s="47" t="s">
+        <v>131</v>
+      </c>
+      <c r="W42">
+        <v>711</v>
+      </c>
+      <c r="X42">
+        <v>2184</v>
+      </c>
+      <c r="Y42">
+        <v>1129</v>
+      </c>
+      <c r="Z42">
+        <v>1920</v>
+      </c>
+      <c r="AA42">
+        <v>2201</v>
+      </c>
+      <c r="AB42">
+        <v>2493</v>
+      </c>
+      <c r="AC42">
+        <v>4910</v>
+      </c>
+      <c r="AD42" s="7">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="AE42">
+        <v>1828</v>
+      </c>
+    </row>
+    <row r="43" spans="21:31" x14ac:dyDescent="0.35">
+      <c r="U43">
+        <v>30</v>
+      </c>
+      <c r="V43" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="W43">
+        <v>187</v>
+      </c>
+      <c r="X43">
+        <v>1512</v>
+      </c>
+      <c r="Y43">
+        <v>855</v>
+      </c>
+      <c r="Z43">
+        <v>1254</v>
+      </c>
+      <c r="AA43">
+        <v>1466</v>
+      </c>
+      <c r="AB43">
+        <v>1737</v>
+      </c>
+      <c r="AC43">
+        <v>3394</v>
+      </c>
+      <c r="AD43" s="7">
+        <f t="shared" si="5"/>
+        <v>0.6660608814175375</v>
+      </c>
+      <c r="AE43">
+        <v>1862</v>
+      </c>
+    </row>
+    <row r="44" spans="21:31" x14ac:dyDescent="0.35">
+      <c r="U44">
         <v>100</v>
       </c>
-      <c r="V28">
-        <v>1296</v>
-      </c>
-      <c r="W28">
-        <v>875</v>
-      </c>
-      <c r="X28">
-        <v>1130</v>
-      </c>
-      <c r="Y28">
-        <v>1236</v>
-      </c>
-      <c r="Z28">
-        <v>1398</v>
-      </c>
-      <c r="AA28">
-        <v>2857</v>
-      </c>
-      <c r="AB28" s="7">
-        <f t="shared" si="2"/>
-        <v>0.70792880258899671</v>
-      </c>
-      <c r="AC28">
-        <f t="shared" si="3"/>
-        <v>2.3114886731391584</v>
+      <c r="V44" s="47" t="s">
+        <v>132</v>
+      </c>
+      <c r="W44">
+        <v>117</v>
+      </c>
+      <c r="X44">
+        <v>1254</v>
+      </c>
+      <c r="Y44">
+        <v>737</v>
+      </c>
+      <c r="Z44">
+        <v>1064</v>
+      </c>
+      <c r="AA44">
+        <v>1217</v>
+      </c>
+      <c r="AB44">
+        <v>1496</v>
+      </c>
+      <c r="AC44">
+        <v>2022</v>
+      </c>
+      <c r="AD44" s="7">
+        <f t="shared" si="5"/>
+        <v>0.55293048614266238</v>
+      </c>
+      <c r="AE44">
+        <v>216</v>
       </c>
     </row>
-    <row r="29" spans="21:29" x14ac:dyDescent="0.4">
-      <c r="U29" s="20" t="s">
-        <v>59</v>
-      </c>
-      <c r="V29">
+    <row r="45" spans="21:31" x14ac:dyDescent="0.35">
+      <c r="U45">
+        <v>300</v>
+      </c>
+      <c r="V45" s="47" t="s">
+        <v>133</v>
+      </c>
+      <c r="W45">
+        <v>63</v>
+      </c>
+      <c r="X45">
+        <v>1045</v>
+      </c>
+      <c r="Y45">
+        <v>730</v>
+      </c>
+      <c r="Z45">
+        <v>865</v>
+      </c>
+      <c r="AA45">
+        <v>990</v>
+      </c>
+      <c r="AB45">
+        <v>1206</v>
+      </c>
+      <c r="AC45">
+        <v>1868</v>
+      </c>
+      <c r="AD45" s="7">
+        <f t="shared" si="5"/>
+        <v>0.44979554747841888</v>
+      </c>
+      <c r="AE45">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="46" spans="21:31" x14ac:dyDescent="0.35">
+      <c r="U46">
         <v>1000</v>
       </c>
-      <c r="W29">
-        <v>634</v>
-      </c>
-      <c r="X29">
-        <v>927</v>
-      </c>
-      <c r="Y29">
-        <v>1016</v>
-      </c>
-      <c r="Z29">
-        <v>1165</v>
-      </c>
-      <c r="AA29">
-        <v>1396</v>
-      </c>
-      <c r="AB29" s="7">
-        <f t="shared" si="2"/>
-        <v>0.62401574803149606</v>
-      </c>
-      <c r="AC29">
-        <f t="shared" si="3"/>
-        <v>1.3740157480314961</v>
+      <c r="V46" s="47" t="s">
+        <v>134</v>
+      </c>
+      <c r="W46">
+        <v>5</v>
+      </c>
+      <c r="X46">
+        <v>772</v>
+      </c>
+      <c r="Y46">
+        <v>633</v>
+      </c>
+      <c r="Z46">
+        <v>670</v>
+      </c>
+      <c r="AA46">
+        <v>777</v>
+      </c>
+      <c r="AB46">
+        <v>893</v>
+      </c>
+      <c r="AC46">
+        <v>1001</v>
+      </c>
+      <c r="AD46" s="7">
+        <f t="shared" si="5"/>
+        <v>0.35302135393003181</v>
+      </c>
+      <c r="AE46">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="AE41:AE46">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="W41:W46">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -8276,19 +11004,19 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.15234375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.15234375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.921875" customWidth="1"/>
-    <col min="4" max="4" width="43.53515625" customWidth="1"/>
-    <col min="5" max="5" width="41.53515625" customWidth="1"/>
+    <col min="1" max="1" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.81640625" customWidth="1"/>
+    <col min="4" max="4" width="43.54296875" customWidth="1"/>
+    <col min="5" max="5" width="41.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
@@ -8301,7 +11029,7 @@
       <c r="D1" s="6"/>
       <c r="E1" s="6"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>43</v>
       </c>
@@ -8314,7 +11042,7 @@
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>48</v>
       </c>
@@ -8325,7 +11053,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>51</v>
       </c>
@@ -8337,7 +11065,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>82</v>
       </c>
@@ -8348,21 +11076,32 @@
         <v>84</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="11"/>
       <c r="B10" s="12" t="s">
         <v>10</v>
       </c>
       <c r="C10" s="13"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="11"/>
       <c r="B11" s="13" t="s">
         <v>11</v>
       </c>
       <c r="C11" s="13"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="15" t="s">
         <v>12</v>
       </c>
@@ -8371,7 +11110,7 @@
       </c>
       <c r="C12" s="16"/>
     </row>
-    <row r="13" spans="1:5" ht="23.15" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:5" ht="23" x14ac:dyDescent="0.35">
       <c r="A13" s="15" t="s">
         <v>15</v>
       </c>
@@ -8382,7 +11121,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="23.15" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:5" ht="23" x14ac:dyDescent="0.35">
       <c r="A14" s="15" t="s">
         <v>18</v>
       </c>
@@ -8393,7 +11132,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="34.75" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:5" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A15" s="15" t="s">
         <v>21</v>
       </c>
@@ -8404,7 +11143,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="34.75" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:5" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A16" s="15" t="s">
         <v>24</v>
       </c>
@@ -8415,7 +11154,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="34.75" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:3" ht="34.5" x14ac:dyDescent="0.35">
       <c r="A17" s="15" t="s">
         <v>27</v>
       </c>
@@ -8426,7 +11165,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="46.3" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:3" ht="46" x14ac:dyDescent="0.35">
       <c r="A18" s="15" t="s">
         <v>30</v>
       </c>
@@ -8437,7 +11176,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="46.3" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:3" ht="46" x14ac:dyDescent="0.35">
       <c r="A19" s="15" t="s">
         <v>33</v>
       </c>
@@ -8448,7 +11187,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="69.45" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:3" ht="71" x14ac:dyDescent="0.35">
       <c r="A20" s="18" t="s">
         <v>36</v>
       </c>
@@ -8464,6 +11203,7 @@
     <hyperlink ref="C2" r:id="rId1"/>
     <hyperlink ref="C3" r:id="rId2"/>
     <hyperlink ref="C5" r:id="rId3"/>
+    <hyperlink ref="C6" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>